<commit_message>
~Increased grammar set size
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\GitHub\auslan-translation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECE7F09-49B3-4612-8F12-2A4AB1F9E5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAF7C2C-D043-4C63-ACA6-660A845401AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2130" windowWidth="16440" windowHeight="29040" activeTab="2" xr2:uid="{2BBB440E-AEF7-4CB8-B155-5AEF60BC9E1F}"/>
   </bookViews>
@@ -733,7 +733,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>Epoch</t>
   </si>
@@ -832,6 +832,9 @@
   </si>
   <si>
     <t>vocab: 6,808, grammar: 50,000</t>
+  </si>
+  <si>
+    <t>vocab: 6,808, grammar: 225,000</t>
   </si>
 </sst>
 </file>
@@ -40554,7 +40557,7 @@
   <dimension ref="A1:AL243"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111:E111"/>
+      <selection activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42878,7 +42881,7 @@
         <v>0.29276000000000002</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -42901,7 +42904,7 @@
         <v>0.29305999999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -42924,7 +42927,7 @@
         <v>0.29305999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -42947,7 +42950,7 @@
         <v>0.29246</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -42970,7 +42973,7 @@
         <v>0.29252</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -42993,7 +42996,7 @@
         <v>0.29239999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -43016,7 +43019,7 @@
         <v>0.29252</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -43039,7 +43042,7 @@
         <v>0.29239999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -43062,7 +43065,7 @@
         <v>0.29233999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -43085,7 +43088,7 @@
         <v>0.29258000000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -43108,7 +43111,7 @@
         <v>0.29227999999999998</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -43131,7 +43134,7 @@
         <v>0.29215999999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -43154,7 +43157,7 @@
         <v>0.29169</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -43177,7 +43180,7 @@
         <v>0.29204999999999998</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -43200,7 +43203,7 @@
         <v>0.29210999999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -43223,12 +43226,18 @@
         <v>0.29175000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
       <c r="F112" s="5"/>
       <c r="G112" s="15"/>
+      <c r="I112" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J112" s="1">
+        <v>4088</v>
+      </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">

</xml_diff>

<commit_message>
~Increased training dataset size
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\GitHub\auslan-translation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAF7C2C-D043-4C63-ACA6-660A845401AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F9817B-0D35-4C5D-8EB3-194732864ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2130" windowWidth="16440" windowHeight="29040" activeTab="2" xr2:uid="{2BBB440E-AEF7-4CB8-B155-5AEF60BC9E1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{2BBB440E-AEF7-4CB8-B155-5AEF60BC9E1F}"/>
   </bookViews>
   <sheets>
     <sheet name="pure_noise" sheetId="1" r:id="rId1"/>
@@ -920,7 +920,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -954,17 +954,14 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4911,6 +4908,66 @@
                 <c:pt idx="57">
                   <c:v>2.2393800000000001</c:v>
                 </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.2768290000000002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.206423</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.1572119999999999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.1006399999999998</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.0472929999999998</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.996575</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.943973</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.898674</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.850266</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.810292</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.7680119999999999</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.7273320000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.6910130000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.66534</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.624811</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.5935550000000001</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.564867</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.535596</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.5074129999999999</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.487182</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5510,6 +5567,66 @@
                 <c:pt idx="57">
                   <c:v>2.4225720000000002</c:v>
                 </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.45736</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.3794900000000001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.3281679999999998</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.272418</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.2126030000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.1616520000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.11368</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.0626929999999999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.0109560000000002</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.969846</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.928758</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.88646</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.8467819999999999</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.821267</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.7763949999999999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.744505</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.7144900000000001</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.686345</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.6564399999999999</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.633095</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6095,6 +6212,66 @@
                 <c:pt idx="57">
                   <c:v>2.5972140000000001</c:v>
                 </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.6415500000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.5597789999999998</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.504146</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.4449429999999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.390631</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.3363119999999999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.2870210000000002</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.2346840000000001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.186982</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.1412610000000001</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.0956969999999999</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.0549529999999998</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.0123470000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.9874210000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.942218</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.9077519999999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.8747750000000001</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.8488910000000001</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.8162970000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.793639</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6679,6 +6856,66 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>2.421732</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.4611109999999998</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.3846820000000002</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.3319420000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.2774030000000001</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.2231830000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.1700309999999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.1198630000000001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.0716489999999999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.0239440000000002</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.980639</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.939012</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.8985479999999999</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.8600099999999999</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.83436</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.790853</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.759509</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.7281489999999999</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.702002</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.6731590000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.6503410000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7295,6 +7532,66 @@
                 <c:pt idx="57">
                   <c:v>0.68376999999999999</c:v>
                 </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.58416000000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.58906000000000003</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.59789000000000003</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.60633000000000004</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.61151</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.622</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.62656000000000001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.63310999999999995</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.64005000000000001</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.65280000000000005</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.65917000000000003</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.66525999999999996</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.67012000000000005</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.67554999999999998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.68342000000000003</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.68471000000000004</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.68647999999999998</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.69154000000000004</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.69460999999999995</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.68942999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7881,6 +8178,66 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>0.29175000000000001</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9.4070000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>9.4490000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>9.4810000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>9.4839999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>9.6339999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9.6689999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9.7729999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9.8150000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>9.9930000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.10037</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.10044</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.10153</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.10194</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.10321</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.10261000000000001</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.10231</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.10384</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.10440000000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.1038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -40556,8 +40913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FC3B5E-94BE-4999-BCE6-46D71699FA22}">
   <dimension ref="A1:AL243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J102" sqref="J102"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB59" sqref="AB59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40616,10 +40973,10 @@
       <c r="E2" s="9">
         <v>4.8840560000000002</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="4">
         <v>0.39867999999999998</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -40648,10 +41005,10 @@
       <c r="E3" s="9">
         <v>4.4829869999999996</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="4">
         <v>0.39874999999999999</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="AL3" t="s">
@@ -40674,10 +41031,10 @@
       <c r="E4" s="9">
         <v>4.398917</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="4">
         <v>0.39896999999999999</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>6.2E-4</v>
       </c>
     </row>
@@ -40697,10 +41054,10 @@
       <c r="E5" s="9">
         <v>4.3600029999999999</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="4">
         <v>0.39923999999999998</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <v>8.4999999999999995E-4</v>
       </c>
     </row>
@@ -40720,10 +41077,10 @@
       <c r="E6" s="9">
         <v>4.2999470000000004</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="4">
         <v>0.40006000000000003</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>2.14E-3</v>
       </c>
     </row>
@@ -40743,10 +41100,10 @@
       <c r="E7" s="9">
         <v>4.1751820000000004</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="4">
         <v>0.40588000000000002</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>1.057E-2</v>
       </c>
     </row>
@@ -40766,10 +41123,10 @@
       <c r="E8" s="9">
         <v>3.902212</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="4">
         <v>0.4345</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <v>3.7909999999999999E-2</v>
       </c>
     </row>
@@ -40789,10 +41146,10 @@
       <c r="E9" s="9">
         <v>3.4164530000000002</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="4">
         <v>0.50804000000000005</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <v>8.795E-2</v>
       </c>
     </row>
@@ -40812,10 +41169,10 @@
       <c r="E10" s="9">
         <v>3.2851439999999998</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="4">
         <v>0.63344</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <v>0.16103999999999999</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -40841,10 +41198,10 @@
       <c r="E11" s="9">
         <v>2.6001210000000001</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="4">
         <v>0.75090999999999997</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <v>0.25348999999999999</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -40870,10 +41227,10 @@
       <c r="E12" s="9">
         <v>2.0049229999999998</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="4">
         <v>0.79549999999999998</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>0.31401000000000001</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -40899,10 +41256,10 @@
       <c r="E13" s="9">
         <v>1.5471699999999999</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="4">
         <v>0.81933</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <v>0.35058</v>
       </c>
     </row>
@@ -40922,10 +41279,10 @@
       <c r="E14" s="9">
         <v>1.567434</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="4">
         <v>0.83350000000000002</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <v>0.37670999999999999</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -40951,10 +41308,10 @@
       <c r="E15" s="9">
         <v>1.226024</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="4">
         <v>0.86016000000000004</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="13">
         <v>0.42331999999999997</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -40980,10 +41337,10 @@
       <c r="E16" s="9">
         <v>0.94228400000000001</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="4">
         <v>0.87619000000000002</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <v>0.46068999999999999</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -41009,10 +41366,10 @@
       <c r="E17" s="9">
         <v>0.74954399999999999</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="4">
         <v>0.87146000000000001</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <v>0.36574000000000001</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -41038,10 +41395,10 @@
       <c r="E18" s="9">
         <v>0.64746599999999999</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="4">
         <v>0.87917000000000001</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <v>0.38834000000000002</v>
       </c>
     </row>
@@ -41061,10 +41418,10 @@
       <c r="E19" s="9">
         <v>0.57961700000000005</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="4">
         <v>0.88180000000000003</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <v>0.39065</v>
       </c>
     </row>
@@ -41084,10 +41441,10 @@
       <c r="E20" s="9">
         <v>0.52724300000000002</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="4">
         <v>0.88353999999999999</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <v>0.39577000000000001</v>
       </c>
     </row>
@@ -41107,10 +41464,10 @@
       <c r="E21" s="9">
         <v>0.49156499999999997</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="4">
         <v>0.88395000000000001</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <v>0.39800999999999997</v>
       </c>
     </row>
@@ -41130,10 +41487,10 @@
       <c r="E22" s="9">
         <v>0.460924</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="4">
         <v>0.88536000000000004</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="13">
         <v>0.39922999999999997</v>
       </c>
     </row>
@@ -41153,10 +41510,10 @@
       <c r="E23" s="9">
         <v>0.439581</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="4">
         <v>0.88573999999999997</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="13">
         <v>0.40359</v>
       </c>
     </row>
@@ -41176,10 +41533,10 @@
       <c r="E24" s="9">
         <v>0.42158699999999999</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="4">
         <v>0.88734000000000002</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <v>0.40601999999999999</v>
       </c>
     </row>
@@ -41199,10 +41556,10 @@
       <c r="E25" s="9">
         <v>0.40392899999999998</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="4">
         <v>0.88776999999999995</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <v>0.40647</v>
       </c>
     </row>
@@ -41222,10 +41579,10 @@
       <c r="E26" s="9">
         <v>0.38692700000000002</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="4">
         <v>0.88741999999999999</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <v>0.40608</v>
       </c>
     </row>
@@ -41245,10 +41602,10 @@
       <c r="E27" s="9">
         <v>0.37537700000000002</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="4">
         <v>0.88844000000000001</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <v>0.40889999999999999</v>
       </c>
     </row>
@@ -41268,10 +41625,10 @@
       <c r="E28" s="9">
         <v>0.36859599999999998</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="4">
         <v>0.88859999999999995</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="13">
         <v>0.40788000000000002</v>
       </c>
     </row>
@@ -41291,10 +41648,10 @@
       <c r="E29" s="9">
         <v>0.35731600000000002</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="4">
         <v>0.88997999999999999</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="13">
         <v>0.41114000000000001</v>
       </c>
     </row>
@@ -41314,10 +41671,10 @@
       <c r="E30" s="9">
         <v>0.34926600000000002</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="4">
         <v>0.89000999999999997</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="13">
         <v>0.41222999999999999</v>
       </c>
     </row>
@@ -41337,10 +41694,10 @@
       <c r="E31" s="9">
         <v>0.341003</v>
       </c>
-      <c r="F31" s="13">
+      <c r="F31" s="4">
         <v>0.88976</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="13">
         <v>0.41326000000000002</v>
       </c>
     </row>
@@ -41360,10 +41717,10 @@
       <c r="E32" s="9">
         <v>0.33349400000000001</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="4">
         <v>0.89059999999999995</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="13">
         <v>0.41504999999999997</v>
       </c>
     </row>
@@ -41383,10 +41740,10 @@
       <c r="E33" s="9">
         <v>0.33015</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="4">
         <v>0.88966999999999996</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="13">
         <v>0.41076000000000001</v>
       </c>
     </row>
@@ -41406,10 +41763,10 @@
       <c r="E34" s="9">
         <v>0.32429400000000003</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="4">
         <v>0.88985000000000003</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="13">
         <v>0.41088999999999998</v>
       </c>
     </row>
@@ -41429,10 +41786,10 @@
       <c r="E35" s="9">
         <v>0.31931199999999998</v>
       </c>
-      <c r="F35" s="13">
+      <c r="F35" s="4">
         <v>0.89027000000000001</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="13">
         <v>0.41415000000000002</v>
       </c>
     </row>
@@ -41452,10 +41809,10 @@
       <c r="E36" s="9">
         <v>0.313189</v>
       </c>
-      <c r="F36" s="13">
+      <c r="F36" s="4">
         <v>0.89015</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="13">
         <v>0.41102</v>
       </c>
     </row>
@@ -41475,10 +41832,10 @@
       <c r="E37" s="9">
         <v>0.30964999999999998</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="4">
         <v>0.90169999999999995</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="13">
         <v>0.52727000000000002</v>
       </c>
       <c r="I37" s="1" t="s">
@@ -41504,10 +41861,10 @@
       <c r="E38" s="9">
         <v>5.8677799999999998</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F38" s="4">
         <v>0.57677999999999996</v>
       </c>
-      <c r="G38" s="15">
+      <c r="G38" s="6">
         <v>0.32179000000000002</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -41533,10 +41890,10 @@
       <c r="E39" s="9">
         <v>4.9511510000000003</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F39" s="4">
         <v>0.60602</v>
       </c>
-      <c r="G39" s="15">
+      <c r="G39" s="6">
         <v>0.32340000000000002</v>
       </c>
     </row>
@@ -41556,10 +41913,10 @@
       <c r="E40" s="9">
         <v>4.4768660000000002</v>
       </c>
-      <c r="F40" s="13">
+      <c r="F40" s="4">
         <v>0.62755000000000005</v>
       </c>
-      <c r="G40" s="15">
+      <c r="G40" s="6">
         <v>0.32435000000000003</v>
       </c>
     </row>
@@ -41579,10 +41936,10 @@
       <c r="E41" s="9">
         <v>4.0912649999999999</v>
       </c>
-      <c r="F41" s="13">
+      <c r="F41" s="4">
         <v>0.64344999999999997</v>
       </c>
-      <c r="G41" s="15">
+      <c r="G41" s="6">
         <v>0.32506000000000002</v>
       </c>
     </row>
@@ -41602,10 +41959,10 @@
       <c r="E42" s="9">
         <v>3.7926479999999998</v>
       </c>
-      <c r="F42" s="13">
+      <c r="F42" s="4">
         <v>0.66274999999999995</v>
       </c>
-      <c r="G42" s="15">
+      <c r="G42" s="6">
         <v>0.32618999999999998</v>
       </c>
     </row>
@@ -41625,10 +41982,10 @@
       <c r="E43" s="9">
         <v>3.555688</v>
       </c>
-      <c r="F43" s="13">
+      <c r="F43" s="4">
         <v>0.68184</v>
       </c>
-      <c r="G43" s="15">
+      <c r="G43" s="6">
         <v>0.32702999999999999</v>
       </c>
     </row>
@@ -41648,10 +42005,10 @@
       <c r="E44" s="9">
         <v>3.370355</v>
       </c>
-      <c r="F44" s="13">
+      <c r="F44" s="4">
         <v>0.69489999999999996</v>
       </c>
-      <c r="G44" s="15">
+      <c r="G44" s="6">
         <v>0.32702999999999999</v>
       </c>
     </row>
@@ -41671,10 +42028,10 @@
       <c r="E45" s="9">
         <v>3.2167509999999999</v>
       </c>
-      <c r="F45" s="13">
+      <c r="F45" s="4">
         <v>0.68949000000000005</v>
       </c>
-      <c r="G45" s="15">
+      <c r="G45" s="6">
         <v>0.32690999999999998</v>
       </c>
     </row>
@@ -41694,10 +42051,10 @@
       <c r="E46" s="9">
         <v>3.0860050000000001</v>
       </c>
-      <c r="F46" s="13">
+      <c r="F46" s="4">
         <v>0.71108000000000005</v>
       </c>
-      <c r="G46" s="15">
+      <c r="G46" s="6">
         <v>0.32756000000000002</v>
       </c>
     </row>
@@ -41717,10 +42074,10 @@
       <c r="E47" s="9">
         <v>3.0693640000000002</v>
       </c>
-      <c r="F47" s="13">
+      <c r="F47" s="4">
         <v>0.71986000000000006</v>
       </c>
-      <c r="G47" s="13">
+      <c r="G47" s="4">
         <v>0.32804</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -41746,10 +42103,10 @@
       <c r="E48" s="9">
         <v>2.8812090000000001</v>
       </c>
-      <c r="F48" s="13">
+      <c r="F48" s="4">
         <v>0.7056</v>
       </c>
-      <c r="G48" s="13">
+      <c r="G48" s="4">
         <v>0.32643</v>
       </c>
     </row>
@@ -41769,10 +42126,10 @@
       <c r="E49" s="9">
         <v>2.7415419999999999</v>
       </c>
-      <c r="F49" s="13">
+      <c r="F49" s="4">
         <v>0.72377000000000002</v>
       </c>
-      <c r="G49" s="13">
+      <c r="G49" s="4">
         <v>0.32715</v>
       </c>
     </row>
@@ -41792,10 +42149,10 @@
       <c r="E50" s="9">
         <v>2.6178379999999999</v>
       </c>
-      <c r="F50" s="13">
+      <c r="F50" s="4">
         <v>0.72721999999999998</v>
       </c>
-      <c r="G50" s="13">
+      <c r="G50" s="4">
         <v>0.32727000000000001</v>
       </c>
     </row>
@@ -41815,10 +42172,10 @@
       <c r="E51" s="9">
         <v>2.4984030000000002</v>
       </c>
-      <c r="F51" s="13">
+      <c r="F51" s="4">
         <v>0.73680999999999996</v>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="4">
         <v>0.32636999999999999</v>
       </c>
     </row>
@@ -41838,10 +42195,10 @@
       <c r="E52" s="9">
         <v>2.3897789999999999</v>
       </c>
-      <c r="F52" s="13">
+      <c r="F52" s="4">
         <v>0.74934999999999996</v>
       </c>
-      <c r="G52" s="13">
+      <c r="G52" s="4">
         <v>0.32601999999999998</v>
       </c>
     </row>
@@ -41861,10 +42218,10 @@
       <c r="E53" s="9">
         <v>2.2889409999999999</v>
       </c>
-      <c r="F53" s="13">
+      <c r="F53" s="4">
         <v>0.75416000000000005</v>
       </c>
-      <c r="G53" s="13">
+      <c r="G53" s="4">
         <v>0.32590000000000002</v>
       </c>
     </row>
@@ -41884,10 +42241,10 @@
       <c r="E54" s="9">
         <v>6.0799709999999996</v>
       </c>
-      <c r="F54" s="13">
+      <c r="F54" s="4">
         <v>0.48485</v>
       </c>
-      <c r="G54" s="15">
+      <c r="G54" s="6">
         <v>0.30924000000000001</v>
       </c>
       <c r="I54" s="1" t="s">
@@ -41913,10 +42270,10 @@
       <c r="E55" s="9">
         <v>5.461576</v>
       </c>
-      <c r="F55" s="13">
+      <c r="F55" s="4">
         <v>0.48937999999999998</v>
       </c>
-      <c r="G55" s="15">
+      <c r="G55" s="6">
         <v>0.30829000000000001</v>
       </c>
     </row>
@@ -41936,10 +42293,10 @@
       <c r="E56" s="9">
         <v>5.2224570000000003</v>
       </c>
-      <c r="F56" s="13">
+      <c r="F56" s="4">
         <v>0.49103999999999998</v>
       </c>
-      <c r="G56" s="15">
+      <c r="G56" s="6">
         <v>0.30364999999999998</v>
       </c>
     </row>
@@ -41959,10 +42316,10 @@
       <c r="E57" s="9">
         <v>5.0895619999999999</v>
       </c>
-      <c r="F57" s="13">
+      <c r="F57" s="4">
         <v>0.48948999999999998</v>
       </c>
-      <c r="G57" s="15">
+      <c r="G57" s="6">
         <v>0.29103000000000001</v>
       </c>
     </row>
@@ -41982,10 +42339,10 @@
       <c r="E58" s="9">
         <v>4.9959600000000002</v>
       </c>
-      <c r="F58" s="13">
+      <c r="F58" s="4">
         <v>0.48815999999999998</v>
       </c>
-      <c r="G58" s="15">
+      <c r="G58" s="6">
         <v>0.27728999999999998</v>
       </c>
     </row>
@@ -42005,10 +42362,10 @@
       <c r="E59" s="9">
         <v>4.9174600000000002</v>
       </c>
-      <c r="F59" s="13">
+      <c r="F59" s="4">
         <v>0.49278</v>
       </c>
-      <c r="G59" s="15">
+      <c r="G59" s="6">
         <v>0.27575</v>
       </c>
     </row>
@@ -42028,10 +42385,10 @@
       <c r="E60" s="9">
         <v>4.8481009999999998</v>
       </c>
-      <c r="F60" s="13">
+      <c r="F60" s="4">
         <v>0.49813000000000002</v>
       </c>
-      <c r="G60" s="15">
+      <c r="G60" s="6">
         <v>0.27848000000000001</v>
       </c>
     </row>
@@ -42051,10 +42408,10 @@
       <c r="E61" s="9">
         <v>4.790254</v>
       </c>
-      <c r="F61" s="13">
+      <c r="F61" s="4">
         <v>0.50221000000000005</v>
       </c>
-      <c r="G61" s="15">
+      <c r="G61" s="6">
         <v>0.28086</v>
       </c>
     </row>
@@ -42074,10 +42431,10 @@
       <c r="E62" s="9">
         <v>4.7402340000000001</v>
       </c>
-      <c r="F62" s="13">
+      <c r="F62" s="4">
         <v>0.50651000000000002</v>
       </c>
-      <c r="G62" s="15">
+      <c r="G62" s="6">
         <v>0.28277000000000002</v>
       </c>
     </row>
@@ -42097,10 +42454,10 @@
       <c r="E63" s="9">
         <v>4.6818520000000001</v>
       </c>
-      <c r="F63" s="13">
+      <c r="F63" s="4">
         <v>0.50968999999999998</v>
       </c>
-      <c r="G63" s="15">
+      <c r="G63" s="6">
         <v>0.28419</v>
       </c>
     </row>
@@ -42120,10 +42477,10 @@
       <c r="E64" s="9">
         <v>4.6311590000000002</v>
       </c>
-      <c r="F64" s="13">
+      <c r="F64" s="4">
         <v>0.51341999999999999</v>
       </c>
-      <c r="G64" s="15">
+      <c r="G64" s="6">
         <v>0.28610000000000002</v>
       </c>
     </row>
@@ -42143,10 +42500,10 @@
       <c r="E65" s="9">
         <v>4.584568</v>
       </c>
-      <c r="F65" s="13">
+      <c r="F65" s="4">
         <v>0.51402000000000003</v>
       </c>
-      <c r="G65" s="15">
+      <c r="G65" s="6">
         <v>0.28741</v>
       </c>
     </row>
@@ -42166,10 +42523,10 @@
       <c r="E66" s="9">
         <v>4.528181</v>
       </c>
-      <c r="F66" s="13">
+      <c r="F66" s="4">
         <v>0.51737999999999995</v>
       </c>
-      <c r="G66" s="15">
+      <c r="G66" s="6">
         <v>0.28656999999999999</v>
       </c>
     </row>
@@ -42189,10 +42546,10 @@
       <c r="E67" s="9">
         <v>4.4836970000000003</v>
       </c>
-      <c r="F67" s="13">
+      <c r="F67" s="4">
         <v>0.52010999999999996</v>
       </c>
-      <c r="G67" s="15">
+      <c r="G67" s="6">
         <v>0.28621999999999997</v>
       </c>
     </row>
@@ -42212,10 +42569,10 @@
       <c r="E68" s="9">
         <v>4.4373230000000001</v>
       </c>
-      <c r="F68" s="13">
+      <c r="F68" s="4">
         <v>0.52490000000000003</v>
       </c>
-      <c r="G68" s="15">
+      <c r="G68" s="6">
         <v>0.28925000000000001</v>
       </c>
       <c r="I68" s="1" t="s">
@@ -42241,10 +42598,10 @@
       <c r="E69" s="9">
         <v>4.3921250000000001</v>
       </c>
-      <c r="F69" s="13">
+      <c r="F69" s="4">
         <v>0.52878999999999998</v>
       </c>
-      <c r="G69" s="15">
+      <c r="G69" s="6">
         <v>0.29199000000000003</v>
       </c>
     </row>
@@ -42264,10 +42621,10 @@
       <c r="E70" s="9">
         <v>4.3533099999999996</v>
       </c>
-      <c r="F70" s="13">
+      <c r="F70" s="4">
         <v>0.53120999999999996</v>
       </c>
-      <c r="G70" s="15">
+      <c r="G70" s="6">
         <v>0.29431000000000002</v>
       </c>
     </row>
@@ -42287,10 +42644,10 @@
       <c r="E71" s="9">
         <v>4.3161849999999999</v>
       </c>
-      <c r="F71" s="13">
+      <c r="F71" s="4">
         <v>0.53569999999999995</v>
       </c>
-      <c r="G71" s="15">
+      <c r="G71" s="6">
         <v>0.29376999999999998</v>
       </c>
     </row>
@@ -42310,10 +42667,10 @@
       <c r="E72" s="9">
         <v>4.284878</v>
       </c>
-      <c r="F72" s="13">
+      <c r="F72" s="4">
         <v>0.53917999999999999</v>
       </c>
-      <c r="G72" s="15">
+      <c r="G72" s="6">
         <v>0.29454000000000002</v>
       </c>
     </row>
@@ -42333,10 +42690,10 @@
       <c r="E73" s="9">
         <v>4.2352829999999999</v>
       </c>
-      <c r="F73" s="13">
+      <c r="F73" s="4">
         <v>0.54061999999999999</v>
       </c>
-      <c r="G73" s="15">
+      <c r="G73" s="6">
         <v>0.29555999999999999</v>
       </c>
     </row>
@@ -42356,10 +42713,10 @@
       <c r="E74" s="9">
         <v>4.1986100000000004</v>
       </c>
-      <c r="F74" s="13">
+      <c r="F74" s="4">
         <v>0.54457</v>
       </c>
-      <c r="G74" s="15">
+      <c r="G74" s="6">
         <v>0.29603000000000002</v>
       </c>
     </row>
@@ -42379,10 +42736,10 @@
       <c r="E75" s="9">
         <v>4.1598829999999998</v>
       </c>
-      <c r="F75" s="13">
+      <c r="F75" s="4">
         <v>0.54651000000000005</v>
       </c>
-      <c r="G75" s="15">
+      <c r="G75" s="6">
         <v>0.29597000000000001</v>
       </c>
     </row>
@@ -42402,10 +42759,10 @@
       <c r="E76" s="9">
         <v>4.1256539999999999</v>
       </c>
-      <c r="F76" s="13">
+      <c r="F76" s="4">
         <v>0.55054999999999998</v>
       </c>
-      <c r="G76" s="15">
+      <c r="G76" s="6">
         <v>0.29609000000000002</v>
       </c>
     </row>
@@ -42425,10 +42782,10 @@
       <c r="E77" s="9">
         <v>4.0872999999999999</v>
       </c>
-      <c r="F77" s="13">
+      <c r="F77" s="4">
         <v>0.55217000000000005</v>
       </c>
-      <c r="G77" s="15">
+      <c r="G77" s="6">
         <v>0.29657</v>
       </c>
     </row>
@@ -42448,10 +42805,10 @@
       <c r="E78" s="9">
         <v>4.0514469999999996</v>
       </c>
-      <c r="F78" s="13">
+      <c r="F78" s="4">
         <v>0.55610000000000004</v>
       </c>
-      <c r="G78" s="15">
+      <c r="G78" s="6">
         <v>0.29620999999999997</v>
       </c>
       <c r="I78" s="1" t="s">
@@ -42477,10 +42834,10 @@
       <c r="E79" s="9">
         <v>4.0123699999999998</v>
       </c>
-      <c r="F79" s="13">
+      <c r="F79" s="4">
         <v>0.55747999999999998</v>
       </c>
-      <c r="G79" s="15">
+      <c r="G79" s="6">
         <v>0.29620999999999997</v>
       </c>
     </row>
@@ -42500,10 +42857,10 @@
       <c r="E80" s="9">
         <v>3.9861309999999999</v>
       </c>
-      <c r="F80" s="13">
+      <c r="F80" s="4">
         <v>0.56044000000000005</v>
       </c>
-      <c r="G80" s="15">
+      <c r="G80" s="6">
         <v>0.29651</v>
       </c>
     </row>
@@ -42523,10 +42880,10 @@
       <c r="E81" s="9">
         <v>3.938876</v>
       </c>
-      <c r="F81" s="13">
+      <c r="F81" s="4">
         <v>0.56405000000000005</v>
       </c>
-      <c r="G81" s="15">
+      <c r="G81" s="6">
         <v>0.29686000000000001</v>
       </c>
     </row>
@@ -42546,10 +42903,10 @@
       <c r="E82" s="9">
         <v>3.9072589999999998</v>
       </c>
-      <c r="F82" s="13">
+      <c r="F82" s="4">
         <v>0.56869000000000003</v>
       </c>
-      <c r="G82" s="15">
+      <c r="G82" s="6">
         <v>0.29651</v>
       </c>
     </row>
@@ -42569,10 +42926,10 @@
       <c r="E83" s="9">
         <v>3.8498739999999998</v>
       </c>
-      <c r="F83" s="13">
+      <c r="F83" s="4">
         <v>0.57284000000000002</v>
       </c>
-      <c r="G83" s="15">
+      <c r="G83" s="6">
         <v>0.29651</v>
       </c>
     </row>
@@ -42592,10 +42949,10 @@
       <c r="E84" s="9">
         <v>3.792179</v>
       </c>
-      <c r="F84" s="13">
+      <c r="F84" s="4">
         <v>0.57726</v>
       </c>
-      <c r="G84" s="15">
+      <c r="G84" s="6">
         <v>0.29620999999999997</v>
       </c>
     </row>
@@ -42615,10 +42972,10 @@
       <c r="E85" s="9">
         <v>3.7276989999999999</v>
       </c>
-      <c r="F85" s="13">
+      <c r="F85" s="4">
         <v>0.58218000000000003</v>
       </c>
-      <c r="G85" s="15">
+      <c r="G85" s="6">
         <v>0.29566999999999999</v>
       </c>
     </row>
@@ -42638,10 +42995,10 @@
       <c r="E86" s="9">
         <v>3.671081</v>
       </c>
-      <c r="F86" s="13">
+      <c r="F86" s="4">
         <v>0.58750000000000002</v>
       </c>
-      <c r="G86" s="15">
+      <c r="G86" s="6">
         <v>0.29561999999999999</v>
       </c>
     </row>
@@ -42661,10 +43018,10 @@
       <c r="E87" s="9">
         <v>3.6068370000000001</v>
       </c>
-      <c r="F87" s="13">
+      <c r="F87" s="4">
         <v>0.59165999999999996</v>
       </c>
-      <c r="G87" s="15">
+      <c r="G87" s="6">
         <v>0.29532000000000003</v>
       </c>
     </row>
@@ -42684,10 +43041,10 @@
       <c r="E88" s="9">
         <v>3.5477240000000001</v>
       </c>
-      <c r="F88" s="13">
+      <c r="F88" s="4">
         <v>0.59465999999999997</v>
       </c>
-      <c r="G88" s="15">
+      <c r="G88" s="6">
         <v>0.29508000000000001</v>
       </c>
       <c r="I88" s="1" t="s">
@@ -42713,10 +43070,10 @@
       <c r="E89" s="9">
         <v>3.4866760000000001</v>
       </c>
-      <c r="F89" s="13">
+      <c r="F89" s="4">
         <v>0.59836999999999996</v>
       </c>
-      <c r="G89" s="15">
+      <c r="G89" s="6">
         <v>0.29483999999999999</v>
       </c>
     </row>
@@ -42736,10 +43093,10 @@
       <c r="E90" s="9">
         <v>3.4256600000000001</v>
       </c>
-      <c r="F90" s="13">
+      <c r="F90" s="4">
         <v>0.60368999999999995</v>
       </c>
-      <c r="G90" s="15">
+      <c r="G90" s="6">
         <v>0.29459999999999997</v>
       </c>
     </row>
@@ -42759,10 +43116,10 @@
       <c r="E91" s="9">
         <v>3.3618209999999999</v>
       </c>
-      <c r="F91" s="13">
+      <c r="F91" s="4">
         <v>0.60775000000000001</v>
       </c>
-      <c r="G91" s="15">
+      <c r="G91" s="6">
         <v>0.29400999999999999</v>
       </c>
     </row>
@@ -42782,10 +43139,10 @@
       <c r="E92" s="9">
         <v>3.3011889999999999</v>
       </c>
-      <c r="F92" s="13">
+      <c r="F92" s="4">
         <v>0.61436999999999997</v>
       </c>
-      <c r="G92" s="15">
+      <c r="G92" s="6">
         <v>0.29335</v>
       </c>
     </row>
@@ -42805,10 +43162,10 @@
       <c r="E93" s="9">
         <v>3.2442709999999999</v>
       </c>
-      <c r="F93" s="13">
+      <c r="F93" s="4">
         <v>0.61573999999999995</v>
       </c>
-      <c r="G93" s="15">
+      <c r="G93" s="6">
         <v>0.29305999999999999</v>
       </c>
     </row>
@@ -42828,10 +43185,10 @@
       <c r="E94" s="9">
         <v>3.1788430000000001</v>
       </c>
-      <c r="F94" s="13">
+      <c r="F94" s="4">
         <v>0.62033000000000005</v>
       </c>
-      <c r="G94" s="15">
+      <c r="G94" s="6">
         <v>0.29353000000000001</v>
       </c>
     </row>
@@ -42851,10 +43208,10 @@
       <c r="E95" s="9">
         <v>3.1224219999999998</v>
       </c>
-      <c r="F95" s="13">
+      <c r="F95" s="4">
         <v>0.62273999999999996</v>
       </c>
-      <c r="G95" s="15">
+      <c r="G95" s="6">
         <v>0.29311999999999999</v>
       </c>
     </row>
@@ -42874,10 +43231,10 @@
       <c r="E96" s="9">
         <v>3.0646</v>
       </c>
-      <c r="F96" s="13">
+      <c r="F96" s="4">
         <v>0.62829999999999997</v>
       </c>
-      <c r="G96" s="15">
+      <c r="G96" s="6">
         <v>0.29276000000000002</v>
       </c>
     </row>
@@ -42897,10 +43254,10 @@
       <c r="E97" s="9">
         <v>3.0098240000000001</v>
       </c>
-      <c r="F97" s="13">
+      <c r="F97" s="4">
         <v>0.63388999999999995</v>
       </c>
-      <c r="G97" s="15">
+      <c r="G97" s="6">
         <v>0.29305999999999999</v>
       </c>
     </row>
@@ -42920,10 +43277,10 @@
       <c r="E98" s="9">
         <v>2.9539230000000001</v>
       </c>
-      <c r="F98" s="13">
+      <c r="F98" s="4">
         <v>0.63736999999999999</v>
       </c>
-      <c r="G98" s="15">
+      <c r="G98" s="6">
         <v>0.29305999999999999</v>
       </c>
     </row>
@@ -42943,10 +43300,10 @@
       <c r="E99" s="9">
         <v>2.9026800000000001</v>
       </c>
-      <c r="F99" s="13">
+      <c r="F99" s="4">
         <v>0.64068999999999998</v>
       </c>
-      <c r="G99" s="15">
+      <c r="G99" s="6">
         <v>0.29246</v>
       </c>
     </row>
@@ -42966,10 +43323,10 @@
       <c r="E100" s="9">
         <v>2.8507769999999999</v>
       </c>
-      <c r="F100" s="13">
+      <c r="F100" s="4">
         <v>0.64822000000000002</v>
       </c>
-      <c r="G100" s="16">
+      <c r="G100" s="14">
         <v>0.29252</v>
       </c>
     </row>
@@ -42989,10 +43346,10 @@
       <c r="E101" s="9">
         <v>2.8058860000000001</v>
       </c>
-      <c r="F101" s="13">
+      <c r="F101" s="4">
         <v>0.64541000000000004</v>
       </c>
-      <c r="G101" s="16">
+      <c r="G101" s="14">
         <v>0.29239999999999999</v>
       </c>
     </row>
@@ -43015,7 +43372,7 @@
       <c r="F102" s="4">
         <v>0.65546000000000004</v>
       </c>
-      <c r="G102" s="15">
+      <c r="G102" s="6">
         <v>0.29252</v>
       </c>
     </row>
@@ -43038,7 +43395,7 @@
       <c r="F103" s="4">
         <v>0.66019000000000005</v>
       </c>
-      <c r="G103" s="15">
+      <c r="G103" s="6">
         <v>0.29239999999999999</v>
       </c>
     </row>
@@ -43061,7 +43418,7 @@
       <c r="F104" s="4">
         <v>0.65966000000000002</v>
       </c>
-      <c r="G104" s="15">
+      <c r="G104" s="6">
         <v>0.29233999999999999</v>
       </c>
     </row>
@@ -43084,7 +43441,7 @@
       <c r="F105" s="4">
         <v>0.66305000000000003</v>
       </c>
-      <c r="G105" s="15">
+      <c r="G105" s="6">
         <v>0.29258000000000001</v>
       </c>
     </row>
@@ -43107,7 +43464,7 @@
       <c r="F106" s="4">
         <v>0.66571999999999998</v>
       </c>
-      <c r="G106" s="15">
+      <c r="G106" s="6">
         <v>0.29227999999999998</v>
       </c>
     </row>
@@ -43127,10 +43484,10 @@
       <c r="E107" s="9">
         <v>2.5600610000000001</v>
       </c>
-      <c r="F107" s="13">
+      <c r="F107" s="4">
         <v>0.67073000000000005</v>
       </c>
-      <c r="G107" s="15">
+      <c r="G107" s="6">
         <v>0.29215999999999998</v>
       </c>
     </row>
@@ -43150,10 +43507,10 @@
       <c r="E108" s="9">
         <v>2.5236679999999998</v>
       </c>
-      <c r="F108" s="13">
+      <c r="F108" s="4">
         <v>0.67320000000000002</v>
       </c>
-      <c r="G108" s="15">
+      <c r="G108" s="6">
         <v>0.29169</v>
       </c>
     </row>
@@ -43173,10 +43530,10 @@
       <c r="E109" s="9">
         <v>2.485948</v>
       </c>
-      <c r="F109" s="13">
+      <c r="F109" s="4">
         <v>0.67615000000000003</v>
       </c>
-      <c r="G109" s="15">
+      <c r="G109" s="6">
         <v>0.29204999999999998</v>
       </c>
     </row>
@@ -43196,10 +43553,10 @@
       <c r="E110" s="9">
         <v>2.4536359999999999</v>
       </c>
-      <c r="F110" s="13">
+      <c r="F110" s="4">
         <v>0.68020999999999998</v>
       </c>
-      <c r="G110" s="15">
+      <c r="G110" s="6">
         <v>0.29210999999999998</v>
       </c>
     </row>
@@ -43219,10 +43576,10 @@
       <c r="E111" s="9">
         <v>2.421732</v>
       </c>
-      <c r="F111" s="15">
+      <c r="F111" s="6">
         <v>0.68376999999999999</v>
       </c>
-      <c r="G111" s="15">
+      <c r="G111" s="6">
         <v>0.29175000000000001</v>
       </c>
     </row>
@@ -43230,8 +43587,24 @@
       <c r="A112" s="1">
         <v>111</v>
       </c>
-      <c r="F112" s="5"/>
-      <c r="G112" s="15"/>
+      <c r="B112" s="9">
+        <v>2.2768290000000002</v>
+      </c>
+      <c r="C112" s="9">
+        <v>2.45736</v>
+      </c>
+      <c r="D112" s="9">
+        <v>2.6415500000000001</v>
+      </c>
+      <c r="E112" s="9">
+        <v>2.4611109999999998</v>
+      </c>
+      <c r="F112" s="15">
+        <v>0.58416000000000001</v>
+      </c>
+      <c r="G112" s="6">
+        <v>9.4070000000000001E-2</v>
+      </c>
       <c r="I112" s="1" t="s">
         <v>33</v>
       </c>
@@ -43243,918 +43616,1222 @@
       <c r="A113" s="1">
         <v>112</v>
       </c>
-      <c r="F113" s="5"/>
-      <c r="G113" s="15"/>
+      <c r="B113" s="9">
+        <v>2.206423</v>
+      </c>
+      <c r="C113" s="9">
+        <v>2.3794900000000001</v>
+      </c>
+      <c r="D113" s="9">
+        <v>2.5597789999999998</v>
+      </c>
+      <c r="E113" s="9">
+        <v>2.3846820000000002</v>
+      </c>
+      <c r="F113" s="15">
+        <v>0.58906000000000003</v>
+      </c>
+      <c r="G113" s="6">
+        <v>9.4490000000000005E-2</v>
+      </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
-      <c r="F114" s="5"/>
-      <c r="G114" s="15"/>
+      <c r="B114" s="9">
+        <v>2.1572119999999999</v>
+      </c>
+      <c r="C114" s="9">
+        <v>2.3281679999999998</v>
+      </c>
+      <c r="D114" s="9">
+        <v>2.504146</v>
+      </c>
+      <c r="E114" s="9">
+        <v>2.3319420000000002</v>
+      </c>
+      <c r="F114" s="15">
+        <v>0.59789000000000003</v>
+      </c>
+      <c r="G114" s="6">
+        <v>9.4810000000000005E-2</v>
+      </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
-      <c r="F115" s="5"/>
-      <c r="G115" s="15"/>
+      <c r="B115" s="9">
+        <v>2.1006399999999998</v>
+      </c>
+      <c r="C115" s="9">
+        <v>2.272418</v>
+      </c>
+      <c r="D115" s="9">
+        <v>2.4449429999999999</v>
+      </c>
+      <c r="E115" s="9">
+        <v>2.2774030000000001</v>
+      </c>
+      <c r="F115" s="15">
+        <v>0.60633000000000004</v>
+      </c>
+      <c r="G115" s="6">
+        <v>9.4839999999999994E-2</v>
+      </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
-      <c r="F116" s="5"/>
-      <c r="G116" s="15"/>
+      <c r="B116" s="9">
+        <v>2.0472929999999998</v>
+      </c>
+      <c r="C116" s="9">
+        <v>2.2126030000000001</v>
+      </c>
+      <c r="D116" s="9">
+        <v>2.390631</v>
+      </c>
+      <c r="E116" s="9">
+        <v>2.2231830000000001</v>
+      </c>
+      <c r="F116" s="15">
+        <v>0.61151</v>
+      </c>
+      <c r="G116" s="6">
+        <v>9.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
-      <c r="F117" s="5"/>
-      <c r="G117" s="15"/>
+      <c r="B117" s="9">
+        <v>1.996575</v>
+      </c>
+      <c r="C117" s="9">
+        <v>2.1616520000000001</v>
+      </c>
+      <c r="D117" s="9">
+        <v>2.3363119999999999</v>
+      </c>
+      <c r="E117" s="9">
+        <v>2.1700309999999998</v>
+      </c>
+      <c r="F117" s="15">
+        <v>0.622</v>
+      </c>
+      <c r="G117" s="6">
+        <v>9.6339999999999995E-2</v>
+      </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
-      <c r="F118" s="5"/>
-      <c r="G118" s="15"/>
+      <c r="B118" s="9">
+        <v>1.943973</v>
+      </c>
+      <c r="C118" s="9">
+        <v>2.11368</v>
+      </c>
+      <c r="D118" s="9">
+        <v>2.2870210000000002</v>
+      </c>
+      <c r="E118" s="9">
+        <v>2.1198630000000001</v>
+      </c>
+      <c r="F118" s="15">
+        <v>0.62656000000000001</v>
+      </c>
+      <c r="G118" s="6">
+        <v>9.6689999999999998E-2</v>
+      </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
-      <c r="F119" s="5"/>
-      <c r="G119" s="15"/>
+      <c r="B119" s="9">
+        <v>1.898674</v>
+      </c>
+      <c r="C119" s="9">
+        <v>2.0626929999999999</v>
+      </c>
+      <c r="D119" s="9">
+        <v>2.2346840000000001</v>
+      </c>
+      <c r="E119" s="9">
+        <v>2.0716489999999999</v>
+      </c>
+      <c r="F119" s="15">
+        <v>0.63310999999999995</v>
+      </c>
+      <c r="G119" s="6">
+        <v>9.7729999999999997E-2</v>
+      </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
-      <c r="F120" s="5"/>
-      <c r="G120" s="15"/>
+      <c r="B120" s="9">
+        <v>1.850266</v>
+      </c>
+      <c r="C120" s="9">
+        <v>2.0109560000000002</v>
+      </c>
+      <c r="D120" s="9">
+        <v>2.186982</v>
+      </c>
+      <c r="E120" s="9">
+        <v>2.0239440000000002</v>
+      </c>
+      <c r="F120" s="15">
+        <v>0.64005000000000001</v>
+      </c>
+      <c r="G120" s="6">
+        <v>9.8150000000000001E-2</v>
+      </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
-      <c r="F121" s="7"/>
-      <c r="G121" s="15"/>
+      <c r="B121" s="9">
+        <v>1.810292</v>
+      </c>
+      <c r="C121" s="9">
+        <v>1.969846</v>
+      </c>
+      <c r="D121" s="9">
+        <v>2.1412610000000001</v>
+      </c>
+      <c r="E121" s="9">
+        <v>1.980639</v>
+      </c>
+      <c r="F121" s="7">
+        <v>0.65280000000000005</v>
+      </c>
+      <c r="G121" s="6">
+        <v>9.9930000000000005E-2</v>
+      </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
-      <c r="F122" s="5"/>
-      <c r="G122" s="15"/>
+      <c r="B122" s="9">
+        <v>1.7680119999999999</v>
+      </c>
+      <c r="C122" s="9">
+        <v>1.928758</v>
+      </c>
+      <c r="D122" s="9">
+        <v>2.0956969999999999</v>
+      </c>
+      <c r="E122" s="9">
+        <v>1.939012</v>
+      </c>
+      <c r="F122" s="15">
+        <v>0.65917000000000003</v>
+      </c>
+      <c r="G122" s="6">
+        <v>0.10037</v>
+      </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
-      <c r="F123" s="5"/>
-      <c r="G123" s="15"/>
+      <c r="B123" s="9">
+        <v>1.7273320000000001</v>
+      </c>
+      <c r="C123" s="9">
+        <v>1.88646</v>
+      </c>
+      <c r="D123" s="9">
+        <v>2.0549529999999998</v>
+      </c>
+      <c r="E123" s="9">
+        <v>1.8985479999999999</v>
+      </c>
+      <c r="F123" s="15">
+        <v>0.66525999999999996</v>
+      </c>
+      <c r="G123" s="6">
+        <v>0.10044</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
-      <c r="F124" s="5"/>
-      <c r="G124" s="15"/>
+      <c r="B124" s="9">
+        <v>1.6910130000000001</v>
+      </c>
+      <c r="C124" s="9">
+        <v>1.8467819999999999</v>
+      </c>
+      <c r="D124" s="9">
+        <v>2.0123470000000001</v>
+      </c>
+      <c r="E124" s="9">
+        <v>1.8600099999999999</v>
+      </c>
+      <c r="F124" s="15">
+        <v>0.67012000000000005</v>
+      </c>
+      <c r="G124" s="6">
+        <v>0.10153</v>
+      </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
-      <c r="F125" s="5"/>
-      <c r="G125" s="15"/>
+      <c r="B125" s="9">
+        <v>1.66534</v>
+      </c>
+      <c r="C125" s="9">
+        <v>1.821267</v>
+      </c>
+      <c r="D125" s="9">
+        <v>1.9874210000000001</v>
+      </c>
+      <c r="E125" s="9">
+        <v>1.83436</v>
+      </c>
+      <c r="F125" s="15">
+        <v>0.67554999999999998</v>
+      </c>
+      <c r="G125" s="6">
+        <v>0.10194</v>
+      </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
-      <c r="F126" s="5"/>
-      <c r="G126" s="15"/>
+      <c r="B126" s="9">
+        <v>1.624811</v>
+      </c>
+      <c r="C126" s="9">
+        <v>1.7763949999999999</v>
+      </c>
+      <c r="D126" s="9">
+        <v>1.942218</v>
+      </c>
+      <c r="E126" s="9">
+        <v>1.790853</v>
+      </c>
+      <c r="F126" s="15">
+        <v>0.68342000000000003</v>
+      </c>
+      <c r="G126" s="6">
+        <v>0.10321</v>
+      </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
-      <c r="F127" s="5"/>
-      <c r="G127" s="15"/>
+      <c r="B127" s="9">
+        <v>1.5935550000000001</v>
+      </c>
+      <c r="C127" s="9">
+        <v>1.744505</v>
+      </c>
+      <c r="D127" s="9">
+        <v>1.9077519999999999</v>
+      </c>
+      <c r="E127" s="9">
+        <v>1.759509</v>
+      </c>
+      <c r="F127" s="15">
+        <v>0.68471000000000004</v>
+      </c>
+      <c r="G127" s="6">
+        <v>0.10261000000000001</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
-      <c r="F128" s="5"/>
-      <c r="G128" s="15"/>
+      <c r="B128" s="9">
+        <v>1.564867</v>
+      </c>
+      <c r="C128" s="9">
+        <v>1.7144900000000001</v>
+      </c>
+      <c r="D128" s="9">
+        <v>1.8747750000000001</v>
+      </c>
+      <c r="E128" s="9">
+        <v>1.7281489999999999</v>
+      </c>
+      <c r="F128" s="15">
+        <v>0.68647999999999998</v>
+      </c>
+      <c r="G128" s="6">
+        <v>0.10231</v>
+      </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
-      <c r="F129" s="5"/>
-      <c r="G129" s="15"/>
+      <c r="B129" s="9">
+        <v>1.535596</v>
+      </c>
+      <c r="C129" s="9">
+        <v>1.686345</v>
+      </c>
+      <c r="D129" s="9">
+        <v>1.8488910000000001</v>
+      </c>
+      <c r="E129" s="9">
+        <v>1.702002</v>
+      </c>
+      <c r="F129" s="15">
+        <v>0.69154000000000004</v>
+      </c>
+      <c r="G129" s="6">
+        <v>0.10384</v>
+      </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
-      <c r="F130" s="5"/>
-      <c r="G130" s="15"/>
+      <c r="B130" s="9">
+        <v>1.5074129999999999</v>
+      </c>
+      <c r="C130" s="9">
+        <v>1.6564399999999999</v>
+      </c>
+      <c r="D130" s="9">
+        <v>1.8162970000000001</v>
+      </c>
+      <c r="E130" s="9">
+        <v>1.6731590000000001</v>
+      </c>
+      <c r="F130" s="15">
+        <v>0.69460999999999995</v>
+      </c>
+      <c r="G130" s="6">
+        <v>0.10440000000000001</v>
+      </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
-      <c r="F131" s="7"/>
-      <c r="G131" s="15"/>
+      <c r="B131" s="9">
+        <v>1.487182</v>
+      </c>
+      <c r="C131" s="9">
+        <v>1.633095</v>
+      </c>
+      <c r="D131" s="9">
+        <v>1.793639</v>
+      </c>
+      <c r="E131" s="9">
+        <v>1.6503410000000001</v>
+      </c>
+      <c r="F131" s="7">
+        <v>0.68942999999999999</v>
+      </c>
+      <c r="G131" s="6">
+        <v>0.1038</v>
+      </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
       <c r="F132" s="5"/>
-      <c r="G132" s="15"/>
+      <c r="G132" s="6"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
       <c r="F133" s="5"/>
-      <c r="G133" s="15"/>
+      <c r="G133" s="6"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
       <c r="F134" s="5"/>
-      <c r="G134" s="15"/>
+      <c r="G134" s="6"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>134</v>
       </c>
       <c r="F135" s="5"/>
-      <c r="G135" s="15"/>
+      <c r="G135" s="6"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
       <c r="F136" s="5"/>
-      <c r="G136" s="15"/>
+      <c r="G136" s="6"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>136</v>
       </c>
       <c r="F137" s="5"/>
-      <c r="G137" s="15"/>
+      <c r="G137" s="6"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
       <c r="F138" s="5"/>
-      <c r="G138" s="15"/>
+      <c r="G138" s="6"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
       <c r="F139" s="6"/>
-      <c r="G139" s="15"/>
+      <c r="G139" s="6"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
       <c r="F140" s="6"/>
-      <c r="G140" s="15"/>
+      <c r="G140" s="6"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
       <c r="F141" s="7"/>
-      <c r="G141" s="15"/>
+      <c r="G141" s="6"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
       <c r="F142" s="6"/>
-      <c r="G142" s="15"/>
+      <c r="G142" s="6"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
       <c r="F143" s="6"/>
-      <c r="G143" s="15"/>
+      <c r="G143" s="6"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>143</v>
       </c>
       <c r="F144" s="6"/>
-      <c r="G144" s="15"/>
+      <c r="G144" s="6"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
       <c r="F145" s="6"/>
-      <c r="G145" s="15"/>
+      <c r="G145" s="6"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
       <c r="F146" s="6"/>
-      <c r="G146" s="15"/>
+      <c r="G146" s="6"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
       <c r="F147" s="6"/>
-      <c r="G147" s="15"/>
+      <c r="G147" s="6"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
       <c r="F148" s="6"/>
-      <c r="G148" s="15"/>
+      <c r="G148" s="6"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
       <c r="F149" s="6"/>
-      <c r="G149" s="15"/>
+      <c r="G149" s="6"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
       <c r="F150" s="6"/>
-      <c r="G150" s="15"/>
+      <c r="G150" s="6"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
       <c r="F151" s="7"/>
-      <c r="G151" s="15"/>
+      <c r="G151" s="6"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
       <c r="F152" s="6"/>
-      <c r="G152" s="15"/>
+      <c r="G152" s="6"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
       <c r="F153" s="6"/>
-      <c r="G153" s="15"/>
+      <c r="G153" s="6"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
       <c r="F154" s="6"/>
-      <c r="G154" s="15"/>
+      <c r="G154" s="6"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
       <c r="F155" s="6"/>
-      <c r="G155" s="15"/>
+      <c r="G155" s="6"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
       <c r="F156" s="6"/>
-      <c r="G156" s="15"/>
+      <c r="G156" s="6"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
       <c r="F157" s="6"/>
-      <c r="G157" s="15"/>
+      <c r="G157" s="6"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
       <c r="F158" s="6"/>
-      <c r="G158" s="15"/>
+      <c r="G158" s="6"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
       <c r="F159" s="6"/>
-      <c r="G159" s="15"/>
+      <c r="G159" s="6"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
       <c r="F160" s="6"/>
-      <c r="G160" s="15"/>
+      <c r="G160" s="6"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
       <c r="F161" s="7"/>
-      <c r="G161" s="15"/>
+      <c r="G161" s="6"/>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
       <c r="F162" s="6"/>
-      <c r="G162" s="15"/>
+      <c r="G162" s="6"/>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
       <c r="F163" s="6"/>
-      <c r="G163" s="15"/>
+      <c r="G163" s="6"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
       <c r="F164" s="6"/>
-      <c r="G164" s="15"/>
+      <c r="G164" s="6"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
       <c r="F165" s="6"/>
-      <c r="G165" s="15"/>
+      <c r="G165" s="6"/>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
       <c r="F166" s="6"/>
-      <c r="G166" s="15"/>
+      <c r="G166" s="6"/>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
       <c r="F167" s="6"/>
-      <c r="G167" s="15"/>
+      <c r="G167" s="6"/>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
       <c r="F168" s="6"/>
-      <c r="G168" s="15"/>
+      <c r="G168" s="6"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
       <c r="F169" s="6"/>
-      <c r="G169" s="15"/>
+      <c r="G169" s="6"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
       <c r="F170" s="6"/>
-      <c r="G170" s="15"/>
+      <c r="G170" s="6"/>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
       <c r="F171" s="7"/>
-      <c r="G171" s="15"/>
+      <c r="G171" s="6"/>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
       <c r="F172" s="6"/>
-      <c r="G172" s="15"/>
+      <c r="G172" s="6"/>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
       <c r="F173" s="6"/>
-      <c r="G173" s="15"/>
+      <c r="G173" s="6"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
       <c r="F174" s="6"/>
-      <c r="G174" s="15"/>
+      <c r="G174" s="6"/>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
       <c r="F175" s="6"/>
-      <c r="G175" s="15"/>
+      <c r="G175" s="6"/>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
       <c r="F176" s="6"/>
-      <c r="G176" s="15"/>
+      <c r="G176" s="6"/>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>176</v>
       </c>
       <c r="F177" s="6"/>
-      <c r="G177" s="15"/>
+      <c r="G177" s="6"/>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
       <c r="F178" s="6"/>
-      <c r="G178" s="15"/>
+      <c r="G178" s="6"/>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
       <c r="F179" s="6"/>
-      <c r="G179" s="15"/>
+      <c r="G179" s="6"/>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
       <c r="F180" s="6"/>
-      <c r="G180" s="15"/>
+      <c r="G180" s="6"/>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
       <c r="F181" s="7"/>
-      <c r="G181" s="15"/>
+      <c r="G181" s="6"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
       <c r="F182" s="6"/>
-      <c r="G182" s="15"/>
+      <c r="G182" s="6"/>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>182</v>
       </c>
       <c r="F183" s="6"/>
-      <c r="G183" s="15"/>
+      <c r="G183" s="6"/>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
       <c r="F184" s="6"/>
-      <c r="G184" s="15"/>
+      <c r="G184" s="6"/>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>184</v>
       </c>
       <c r="F185" s="6"/>
-      <c r="G185" s="15"/>
+      <c r="G185" s="6"/>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
       <c r="F186" s="6"/>
-      <c r="G186" s="15"/>
+      <c r="G186" s="6"/>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>186</v>
       </c>
       <c r="F187" s="6"/>
-      <c r="G187" s="15"/>
+      <c r="G187" s="6"/>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
       <c r="F188" s="6"/>
-      <c r="G188" s="15"/>
+      <c r="G188" s="6"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>188</v>
       </c>
       <c r="F189" s="6"/>
-      <c r="G189" s="15"/>
+      <c r="G189" s="6"/>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
       <c r="F190" s="6"/>
-      <c r="G190" s="15"/>
+      <c r="G190" s="6"/>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>190</v>
       </c>
       <c r="F191" s="7"/>
-      <c r="G191" s="15"/>
+      <c r="G191" s="6"/>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
       <c r="F192" s="6"/>
-      <c r="G192" s="15"/>
+      <c r="G192" s="6"/>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
       <c r="F193" s="6"/>
-      <c r="G193" s="15"/>
+      <c r="G193" s="6"/>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
       <c r="F194" s="6"/>
-      <c r="G194" s="15"/>
+      <c r="G194" s="6"/>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>194</v>
       </c>
       <c r="F195" s="6"/>
-      <c r="G195" s="15"/>
+      <c r="G195" s="6"/>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
       <c r="F196" s="6"/>
-      <c r="G196" s="15"/>
+      <c r="G196" s="6"/>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
       <c r="F197" s="6"/>
-      <c r="G197" s="15"/>
+      <c r="G197" s="6"/>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
       <c r="F198" s="6"/>
-      <c r="G198" s="15"/>
+      <c r="G198" s="6"/>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>198</v>
       </c>
       <c r="F199" s="6"/>
-      <c r="G199" s="15"/>
+      <c r="G199" s="6"/>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
       <c r="F200" s="6"/>
-      <c r="G200" s="15"/>
+      <c r="G200" s="6"/>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>200</v>
       </c>
       <c r="F201" s="7"/>
-      <c r="G201" s="15"/>
+      <c r="G201" s="6"/>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
       <c r="F202" s="6"/>
-      <c r="G202" s="15"/>
+      <c r="G202" s="6"/>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>202</v>
       </c>
       <c r="F203" s="6"/>
-      <c r="G203" s="15"/>
+      <c r="G203" s="6"/>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
       <c r="F204" s="6"/>
-      <c r="G204" s="15"/>
+      <c r="G204" s="6"/>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>204</v>
       </c>
       <c r="F205" s="6"/>
-      <c r="G205" s="15"/>
+      <c r="G205" s="6"/>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>205</v>
       </c>
       <c r="F206" s="6"/>
-      <c r="G206" s="15"/>
+      <c r="G206" s="6"/>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>206</v>
       </c>
       <c r="F207" s="6"/>
-      <c r="G207" s="15"/>
+      <c r="G207" s="6"/>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>207</v>
       </c>
       <c r="F208" s="6"/>
-      <c r="G208" s="15"/>
+      <c r="G208" s="6"/>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>208</v>
       </c>
       <c r="F209" s="6"/>
-      <c r="G209" s="15"/>
+      <c r="G209" s="6"/>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>209</v>
       </c>
       <c r="F210" s="7"/>
-      <c r="G210" s="15"/>
+      <c r="G210" s="6"/>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>210</v>
       </c>
       <c r="F211" s="7"/>
-      <c r="G211" s="15"/>
+      <c r="G211" s="6"/>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>211</v>
       </c>
       <c r="F212" s="6"/>
-      <c r="G212" s="15"/>
+      <c r="G212" s="6"/>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>212</v>
       </c>
       <c r="F213" s="6"/>
-      <c r="G213" s="15"/>
+      <c r="G213" s="6"/>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>213</v>
       </c>
       <c r="F214" s="6"/>
-      <c r="G214" s="15"/>
+      <c r="G214" s="6"/>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>214</v>
       </c>
       <c r="F215" s="6"/>
-      <c r="G215" s="15"/>
+      <c r="G215" s="6"/>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>215</v>
       </c>
       <c r="F216" s="6"/>
-      <c r="G216" s="15"/>
+      <c r="G216" s="6"/>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>216</v>
       </c>
       <c r="F217" s="6"/>
-      <c r="G217" s="15"/>
+      <c r="G217" s="6"/>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>217</v>
       </c>
       <c r="F218" s="6"/>
-      <c r="G218" s="15"/>
+      <c r="G218" s="6"/>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>218</v>
       </c>
       <c r="F219" s="6"/>
-      <c r="G219" s="15"/>
+      <c r="G219" s="6"/>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>219</v>
       </c>
       <c r="F220" s="6"/>
-      <c r="G220" s="15"/>
+      <c r="G220" s="6"/>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>220</v>
       </c>
       <c r="F221" s="7"/>
-      <c r="G221" s="15"/>
+      <c r="G221" s="6"/>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>221</v>
       </c>
       <c r="F222" s="6"/>
-      <c r="G222" s="15"/>
+      <c r="G222" s="6"/>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>222</v>
       </c>
       <c r="F223" s="6"/>
-      <c r="G223" s="15"/>
+      <c r="G223" s="6"/>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>223</v>
       </c>
       <c r="F224" s="6"/>
-      <c r="G224" s="15"/>
+      <c r="G224" s="6"/>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>224</v>
       </c>
       <c r="F225" s="6"/>
-      <c r="G225" s="15"/>
+      <c r="G225" s="6"/>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>225</v>
       </c>
       <c r="F226" s="6"/>
-      <c r="G226" s="15"/>
+      <c r="G226" s="6"/>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>226</v>
       </c>
       <c r="F227" s="6"/>
-      <c r="G227" s="15"/>
+      <c r="G227" s="6"/>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>227</v>
       </c>
       <c r="F228" s="6"/>
-      <c r="G228" s="15"/>
+      <c r="G228" s="6"/>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>228</v>
       </c>
       <c r="F229" s="6"/>
-      <c r="G229" s="15"/>
+      <c r="G229" s="6"/>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>229</v>
       </c>
       <c r="F230" s="6"/>
-      <c r="G230" s="15"/>
+      <c r="G230" s="6"/>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>230</v>
       </c>
       <c r="F231" s="7"/>
-      <c r="G231" s="15"/>
+      <c r="G231" s="6"/>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>231</v>
       </c>
       <c r="F232" s="6"/>
-      <c r="G232" s="15"/>
+      <c r="G232" s="6"/>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>232</v>
       </c>
       <c r="F233" s="6"/>
-      <c r="G233" s="15"/>
+      <c r="G233" s="6"/>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>233</v>
       </c>
       <c r="F234" s="6"/>
-      <c r="G234" s="15"/>
+      <c r="G234" s="6"/>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>234</v>
       </c>
       <c r="F235" s="6"/>
-      <c r="G235" s="15"/>
+      <c r="G235" s="6"/>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>235</v>
       </c>
       <c r="F236" s="6"/>
-      <c r="G236" s="15"/>
+      <c r="G236" s="6"/>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>236</v>
       </c>
       <c r="F237" s="6"/>
-      <c r="G237" s="15"/>
+      <c r="G237" s="6"/>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>237</v>
       </c>
       <c r="F238" s="6"/>
-      <c r="G238" s="15"/>
+      <c r="G238" s="6"/>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>238</v>
       </c>
       <c r="F239" s="6"/>
-      <c r="G239" s="15"/>
+      <c r="G239" s="6"/>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>239</v>
       </c>
       <c r="F240" s="6"/>
-      <c r="G240" s="15"/>
+      <c r="G240" s="6"/>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>240</v>
       </c>
       <c r="F241" s="6"/>
-      <c r="G241" s="15"/>
+      <c r="G241" s="6"/>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>241</v>
       </c>
       <c r="F242" s="6"/>
-      <c r="G242" s="15"/>
+      <c r="G242" s="6"/>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>242</v>
       </c>
       <c r="F243" s="6"/>
-      <c r="G243" s="15"/>
+      <c r="G243" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
~Trained on larger dataset
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\GitHub\auslan-translation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F9817B-0D35-4C5D-8EB3-194732864ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3955F8-9EDF-46DA-A5F6-F9B8D881B96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{2BBB440E-AEF7-4CB8-B155-5AEF60BC9E1F}"/>
   </bookViews>
@@ -733,7 +733,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t>Epoch</t>
   </si>
@@ -836,6 +836,15 @@
   <si>
     <t>vocab: 6,808, grammar: 225,000</t>
   </si>
+  <si>
+    <t>vocab: 6,808, grammar: 450,000</t>
+  </si>
+  <si>
+    <t>vocab: 6,808, word-masking: 90,000</t>
+  </si>
+  <si>
+    <t>vocab: 6,808, word-masking: 45,000</t>
+  </si>
 </sst>
 </file>
 
@@ -920,7 +929,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -963,6 +972,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4968,6 +4981,12 @@
                 <c:pt idx="77">
                   <c:v>1.487182</c:v>
                 </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.521034</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.4579949999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5627,6 +5646,12 @@
                 <c:pt idx="77">
                   <c:v>1.633095</c:v>
                 </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.679262</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.6021639999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6272,6 +6297,12 @@
                 <c:pt idx="77">
                   <c:v>1.793639</c:v>
                 </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.8647670000000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.763342</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6916,6 +6947,12 @@
                 </c:pt>
                 <c:pt idx="77">
                   <c:v>1.6503410000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.712413</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.6224209999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7592,6 +7629,12 @@
                 <c:pt idx="77">
                   <c:v>0.68942999999999999</c:v>
                 </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.69579999999999997</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.70584999999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8238,6 +8281,12 @@
                 </c:pt>
                 <c:pt idx="77">
                   <c:v>0.1038</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.10402</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.10562000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -40913,8 +40962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FC3B5E-94BE-4999-BCE6-46D71699FA22}">
   <dimension ref="A1:AL243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB59" sqref="AB59"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40973,7 +41022,7 @@
       <c r="E2" s="9">
         <v>4.8840560000000002</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="15">
         <v>0.39867999999999998</v>
       </c>
       <c r="G2" s="13">
@@ -41005,7 +41054,7 @@
       <c r="E3" s="9">
         <v>4.4829869999999996</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="15">
         <v>0.39874999999999999</v>
       </c>
       <c r="G3" s="13">
@@ -41031,7 +41080,7 @@
       <c r="E4" s="9">
         <v>4.398917</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="15">
         <v>0.39896999999999999</v>
       </c>
       <c r="G4" s="13">
@@ -41054,7 +41103,7 @@
       <c r="E5" s="9">
         <v>4.3600029999999999</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="15">
         <v>0.39923999999999998</v>
       </c>
       <c r="G5" s="13">
@@ -41077,7 +41126,7 @@
       <c r="E6" s="9">
         <v>4.2999470000000004</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="15">
         <v>0.40006000000000003</v>
       </c>
       <c r="G6" s="13">
@@ -41100,7 +41149,7 @@
       <c r="E7" s="9">
         <v>4.1751820000000004</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="15">
         <v>0.40588000000000002</v>
       </c>
       <c r="G7" s="13">
@@ -41123,7 +41172,7 @@
       <c r="E8" s="9">
         <v>3.902212</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="15">
         <v>0.4345</v>
       </c>
       <c r="G8" s="13">
@@ -41146,7 +41195,7 @@
       <c r="E9" s="9">
         <v>3.4164530000000002</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="15">
         <v>0.50804000000000005</v>
       </c>
       <c r="G9" s="13">
@@ -41169,7 +41218,7 @@
       <c r="E10" s="9">
         <v>3.2851439999999998</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="15">
         <v>0.63344</v>
       </c>
       <c r="G10" s="13">
@@ -41198,7 +41247,7 @@
       <c r="E11" s="9">
         <v>2.6001210000000001</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="15">
         <v>0.75090999999999997</v>
       </c>
       <c r="G11" s="13">
@@ -41227,7 +41276,7 @@
       <c r="E12" s="9">
         <v>2.0049229999999998</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="15">
         <v>0.79549999999999998</v>
       </c>
       <c r="G12" s="13">
@@ -41256,7 +41305,7 @@
       <c r="E13" s="9">
         <v>1.5471699999999999</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="15">
         <v>0.81933</v>
       </c>
       <c r="G13" s="13">
@@ -41279,7 +41328,7 @@
       <c r="E14" s="9">
         <v>1.567434</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="15">
         <v>0.83350000000000002</v>
       </c>
       <c r="G14" s="13">
@@ -41308,7 +41357,7 @@
       <c r="E15" s="9">
         <v>1.226024</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="15">
         <v>0.86016000000000004</v>
       </c>
       <c r="G15" s="13">
@@ -41337,7 +41386,7 @@
       <c r="E16" s="9">
         <v>0.94228400000000001</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="15">
         <v>0.87619000000000002</v>
       </c>
       <c r="G16" s="13">
@@ -41366,7 +41415,7 @@
       <c r="E17" s="9">
         <v>0.74954399999999999</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="15">
         <v>0.87146000000000001</v>
       </c>
       <c r="G17" s="13">
@@ -41395,7 +41444,7 @@
       <c r="E18" s="9">
         <v>0.64746599999999999</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="15">
         <v>0.87917000000000001</v>
       </c>
       <c r="G18" s="13">
@@ -41418,7 +41467,7 @@
       <c r="E19" s="9">
         <v>0.57961700000000005</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="15">
         <v>0.88180000000000003</v>
       </c>
       <c r="G19" s="13">
@@ -41441,7 +41490,7 @@
       <c r="E20" s="9">
         <v>0.52724300000000002</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="15">
         <v>0.88353999999999999</v>
       </c>
       <c r="G20" s="13">
@@ -41464,7 +41513,7 @@
       <c r="E21" s="9">
         <v>0.49156499999999997</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="15">
         <v>0.88395000000000001</v>
       </c>
       <c r="G21" s="13">
@@ -41487,7 +41536,7 @@
       <c r="E22" s="9">
         <v>0.460924</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="15">
         <v>0.88536000000000004</v>
       </c>
       <c r="G22" s="13">
@@ -41510,7 +41559,7 @@
       <c r="E23" s="9">
         <v>0.439581</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="15">
         <v>0.88573999999999997</v>
       </c>
       <c r="G23" s="13">
@@ -41533,7 +41582,7 @@
       <c r="E24" s="9">
         <v>0.42158699999999999</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="15">
         <v>0.88734000000000002</v>
       </c>
       <c r="G24" s="13">
@@ -41556,7 +41605,7 @@
       <c r="E25" s="9">
         <v>0.40392899999999998</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="15">
         <v>0.88776999999999995</v>
       </c>
       <c r="G25" s="13">
@@ -41579,7 +41628,7 @@
       <c r="E26" s="9">
         <v>0.38692700000000002</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="15">
         <v>0.88741999999999999</v>
       </c>
       <c r="G26" s="13">
@@ -41602,7 +41651,7 @@
       <c r="E27" s="9">
         <v>0.37537700000000002</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="15">
         <v>0.88844000000000001</v>
       </c>
       <c r="G27" s="13">
@@ -41625,7 +41674,7 @@
       <c r="E28" s="9">
         <v>0.36859599999999998</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="15">
         <v>0.88859999999999995</v>
       </c>
       <c r="G28" s="13">
@@ -41648,7 +41697,7 @@
       <c r="E29" s="9">
         <v>0.35731600000000002</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="15">
         <v>0.88997999999999999</v>
       </c>
       <c r="G29" s="13">
@@ -41671,7 +41720,7 @@
       <c r="E30" s="9">
         <v>0.34926600000000002</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="15">
         <v>0.89000999999999997</v>
       </c>
       <c r="G30" s="13">
@@ -41694,7 +41743,7 @@
       <c r="E31" s="9">
         <v>0.341003</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="15">
         <v>0.88976</v>
       </c>
       <c r="G31" s="13">
@@ -41717,7 +41766,7 @@
       <c r="E32" s="9">
         <v>0.33349400000000001</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="15">
         <v>0.89059999999999995</v>
       </c>
       <c r="G32" s="13">
@@ -41740,7 +41789,7 @@
       <c r="E33" s="9">
         <v>0.33015</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="15">
         <v>0.88966999999999996</v>
       </c>
       <c r="G33" s="13">
@@ -41763,7 +41812,7 @@
       <c r="E34" s="9">
         <v>0.32429400000000003</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="15">
         <v>0.88985000000000003</v>
       </c>
       <c r="G34" s="13">
@@ -41786,7 +41835,7 @@
       <c r="E35" s="9">
         <v>0.31931199999999998</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="15">
         <v>0.89027000000000001</v>
       </c>
       <c r="G35" s="13">
@@ -41809,7 +41858,7 @@
       <c r="E36" s="9">
         <v>0.313189</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="15">
         <v>0.89015</v>
       </c>
       <c r="G36" s="13">
@@ -41832,7 +41881,7 @@
       <c r="E37" s="9">
         <v>0.30964999999999998</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="15">
         <v>0.90169999999999995</v>
       </c>
       <c r="G37" s="13">
@@ -41861,14 +41910,14 @@
       <c r="E38" s="9">
         <v>5.8677799999999998</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="15">
         <v>0.57677999999999996</v>
       </c>
       <c r="G38" s="6">
         <v>0.32179000000000002</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="J38" s="1">
         <v>4088</v>
@@ -41890,7 +41939,7 @@
       <c r="E39" s="9">
         <v>4.9511510000000003</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="15">
         <v>0.60602</v>
       </c>
       <c r="G39" s="6">
@@ -41913,7 +41962,7 @@
       <c r="E40" s="9">
         <v>4.4768660000000002</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40" s="15">
         <v>0.62755000000000005</v>
       </c>
       <c r="G40" s="6">
@@ -41936,7 +41985,7 @@
       <c r="E41" s="9">
         <v>4.0912649999999999</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41" s="15">
         <v>0.64344999999999997</v>
       </c>
       <c r="G41" s="6">
@@ -41959,7 +42008,7 @@
       <c r="E42" s="9">
         <v>3.7926479999999998</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F42" s="15">
         <v>0.66274999999999995</v>
       </c>
       <c r="G42" s="6">
@@ -41982,7 +42031,7 @@
       <c r="E43" s="9">
         <v>3.555688</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F43" s="15">
         <v>0.68184</v>
       </c>
       <c r="G43" s="6">
@@ -42005,7 +42054,7 @@
       <c r="E44" s="9">
         <v>3.370355</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="15">
         <v>0.69489999999999996</v>
       </c>
       <c r="G44" s="6">
@@ -42028,7 +42077,7 @@
       <c r="E45" s="9">
         <v>3.2167509999999999</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45" s="15">
         <v>0.68949000000000005</v>
       </c>
       <c r="G45" s="6">
@@ -42051,7 +42100,7 @@
       <c r="E46" s="9">
         <v>3.0860050000000001</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46" s="15">
         <v>0.71108000000000005</v>
       </c>
       <c r="G46" s="6">
@@ -42074,14 +42123,14 @@
       <c r="E47" s="9">
         <v>3.0693640000000002</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47" s="15">
         <v>0.71986000000000006</v>
       </c>
       <c r="G47" s="4">
         <v>0.32804</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J47" s="1">
         <v>4088</v>
@@ -42103,7 +42152,7 @@
       <c r="E48" s="9">
         <v>2.8812090000000001</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F48" s="15">
         <v>0.7056</v>
       </c>
       <c r="G48" s="4">
@@ -42126,7 +42175,7 @@
       <c r="E49" s="9">
         <v>2.7415419999999999</v>
       </c>
-      <c r="F49" s="4">
+      <c r="F49" s="15">
         <v>0.72377000000000002</v>
       </c>
       <c r="G49" s="4">
@@ -42149,7 +42198,7 @@
       <c r="E50" s="9">
         <v>2.6178379999999999</v>
       </c>
-      <c r="F50" s="4">
+      <c r="F50" s="15">
         <v>0.72721999999999998</v>
       </c>
       <c r="G50" s="4">
@@ -42172,7 +42221,7 @@
       <c r="E51" s="9">
         <v>2.4984030000000002</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F51" s="15">
         <v>0.73680999999999996</v>
       </c>
       <c r="G51" s="4">
@@ -42195,7 +42244,7 @@
       <c r="E52" s="9">
         <v>2.3897789999999999</v>
       </c>
-      <c r="F52" s="4">
+      <c r="F52" s="15">
         <v>0.74934999999999996</v>
       </c>
       <c r="G52" s="4">
@@ -42218,7 +42267,7 @@
       <c r="E53" s="9">
         <v>2.2889409999999999</v>
       </c>
-      <c r="F53" s="4">
+      <c r="F53" s="15">
         <v>0.75416000000000005</v>
       </c>
       <c r="G53" s="4">
@@ -42241,7 +42290,7 @@
       <c r="E54" s="9">
         <v>6.0799709999999996</v>
       </c>
-      <c r="F54" s="4">
+      <c r="F54" s="15">
         <v>0.48485</v>
       </c>
       <c r="G54" s="6">
@@ -42270,7 +42319,7 @@
       <c r="E55" s="9">
         <v>5.461576</v>
       </c>
-      <c r="F55" s="4">
+      <c r="F55" s="15">
         <v>0.48937999999999998</v>
       </c>
       <c r="G55" s="6">
@@ -42293,7 +42342,7 @@
       <c r="E56" s="9">
         <v>5.2224570000000003</v>
       </c>
-      <c r="F56" s="4">
+      <c r="F56" s="15">
         <v>0.49103999999999998</v>
       </c>
       <c r="G56" s="6">
@@ -42316,7 +42365,7 @@
       <c r="E57" s="9">
         <v>5.0895619999999999</v>
       </c>
-      <c r="F57" s="4">
+      <c r="F57" s="15">
         <v>0.48948999999999998</v>
       </c>
       <c r="G57" s="6">
@@ -42339,7 +42388,7 @@
       <c r="E58" s="9">
         <v>4.9959600000000002</v>
       </c>
-      <c r="F58" s="4">
+      <c r="F58" s="15">
         <v>0.48815999999999998</v>
       </c>
       <c r="G58" s="6">
@@ -42362,7 +42411,7 @@
       <c r="E59" s="9">
         <v>4.9174600000000002</v>
       </c>
-      <c r="F59" s="4">
+      <c r="F59" s="15">
         <v>0.49278</v>
       </c>
       <c r="G59" s="6">
@@ -42385,7 +42434,7 @@
       <c r="E60" s="9">
         <v>4.8481009999999998</v>
       </c>
-      <c r="F60" s="4">
+      <c r="F60" s="15">
         <v>0.49813000000000002</v>
       </c>
       <c r="G60" s="6">
@@ -42408,7 +42457,7 @@
       <c r="E61" s="9">
         <v>4.790254</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F61" s="15">
         <v>0.50221000000000005</v>
       </c>
       <c r="G61" s="6">
@@ -42431,7 +42480,7 @@
       <c r="E62" s="9">
         <v>4.7402340000000001</v>
       </c>
-      <c r="F62" s="4">
+      <c r="F62" s="15">
         <v>0.50651000000000002</v>
       </c>
       <c r="G62" s="6">
@@ -42454,7 +42503,7 @@
       <c r="E63" s="9">
         <v>4.6818520000000001</v>
       </c>
-      <c r="F63" s="4">
+      <c r="F63" s="15">
         <v>0.50968999999999998</v>
       </c>
       <c r="G63" s="6">
@@ -42477,7 +42526,7 @@
       <c r="E64" s="9">
         <v>4.6311590000000002</v>
       </c>
-      <c r="F64" s="4">
+      <c r="F64" s="15">
         <v>0.51341999999999999</v>
       </c>
       <c r="G64" s="6">
@@ -42500,7 +42549,7 @@
       <c r="E65" s="9">
         <v>4.584568</v>
       </c>
-      <c r="F65" s="4">
+      <c r="F65" s="15">
         <v>0.51402000000000003</v>
       </c>
       <c r="G65" s="6">
@@ -42523,7 +42572,7 @@
       <c r="E66" s="9">
         <v>4.528181</v>
       </c>
-      <c r="F66" s="4">
+      <c r="F66" s="15">
         <v>0.51737999999999995</v>
       </c>
       <c r="G66" s="6">
@@ -42546,7 +42595,7 @@
       <c r="E67" s="9">
         <v>4.4836970000000003</v>
       </c>
-      <c r="F67" s="4">
+      <c r="F67" s="15">
         <v>0.52010999999999996</v>
       </c>
       <c r="G67" s="6">
@@ -42569,7 +42618,7 @@
       <c r="E68" s="9">
         <v>4.4373230000000001</v>
       </c>
-      <c r="F68" s="4">
+      <c r="F68" s="15">
         <v>0.52490000000000003</v>
       </c>
       <c r="G68" s="6">
@@ -42598,7 +42647,7 @@
       <c r="E69" s="9">
         <v>4.3921250000000001</v>
       </c>
-      <c r="F69" s="4">
+      <c r="F69" s="15">
         <v>0.52878999999999998</v>
       </c>
       <c r="G69" s="6">
@@ -42621,7 +42670,7 @@
       <c r="E70" s="9">
         <v>4.3533099999999996</v>
       </c>
-      <c r="F70" s="4">
+      <c r="F70" s="15">
         <v>0.53120999999999996</v>
       </c>
       <c r="G70" s="6">
@@ -42644,7 +42693,7 @@
       <c r="E71" s="9">
         <v>4.3161849999999999</v>
       </c>
-      <c r="F71" s="4">
+      <c r="F71" s="15">
         <v>0.53569999999999995</v>
       </c>
       <c r="G71" s="6">
@@ -42667,7 +42716,7 @@
       <c r="E72" s="9">
         <v>4.284878</v>
       </c>
-      <c r="F72" s="4">
+      <c r="F72" s="15">
         <v>0.53917999999999999</v>
       </c>
       <c r="G72" s="6">
@@ -42690,7 +42739,7 @@
       <c r="E73" s="9">
         <v>4.2352829999999999</v>
       </c>
-      <c r="F73" s="4">
+      <c r="F73" s="15">
         <v>0.54061999999999999</v>
       </c>
       <c r="G73" s="6">
@@ -42713,7 +42762,7 @@
       <c r="E74" s="9">
         <v>4.1986100000000004</v>
       </c>
-      <c r="F74" s="4">
+      <c r="F74" s="15">
         <v>0.54457</v>
       </c>
       <c r="G74" s="6">
@@ -42736,7 +42785,7 @@
       <c r="E75" s="9">
         <v>4.1598829999999998</v>
       </c>
-      <c r="F75" s="4">
+      <c r="F75" s="15">
         <v>0.54651000000000005</v>
       </c>
       <c r="G75" s="6">
@@ -42759,7 +42808,7 @@
       <c r="E76" s="9">
         <v>4.1256539999999999</v>
       </c>
-      <c r="F76" s="4">
+      <c r="F76" s="15">
         <v>0.55054999999999998</v>
       </c>
       <c r="G76" s="6">
@@ -42782,7 +42831,7 @@
       <c r="E77" s="9">
         <v>4.0872999999999999</v>
       </c>
-      <c r="F77" s="4">
+      <c r="F77" s="15">
         <v>0.55217000000000005</v>
       </c>
       <c r="G77" s="6">
@@ -42805,7 +42854,7 @@
       <c r="E78" s="9">
         <v>4.0514469999999996</v>
       </c>
-      <c r="F78" s="4">
+      <c r="F78" s="15">
         <v>0.55610000000000004</v>
       </c>
       <c r="G78" s="6">
@@ -42834,7 +42883,7 @@
       <c r="E79" s="9">
         <v>4.0123699999999998</v>
       </c>
-      <c r="F79" s="4">
+      <c r="F79" s="15">
         <v>0.55747999999999998</v>
       </c>
       <c r="G79" s="6">
@@ -42857,7 +42906,7 @@
       <c r="E80" s="9">
         <v>3.9861309999999999</v>
       </c>
-      <c r="F80" s="4">
+      <c r="F80" s="15">
         <v>0.56044000000000005</v>
       </c>
       <c r="G80" s="6">
@@ -42880,7 +42929,7 @@
       <c r="E81" s="9">
         <v>3.938876</v>
       </c>
-      <c r="F81" s="4">
+      <c r="F81" s="15">
         <v>0.56405000000000005</v>
       </c>
       <c r="G81" s="6">
@@ -42903,7 +42952,7 @@
       <c r="E82" s="9">
         <v>3.9072589999999998</v>
       </c>
-      <c r="F82" s="4">
+      <c r="F82" s="15">
         <v>0.56869000000000003</v>
       </c>
       <c r="G82" s="6">
@@ -42926,7 +42975,7 @@
       <c r="E83" s="9">
         <v>3.8498739999999998</v>
       </c>
-      <c r="F83" s="4">
+      <c r="F83" s="15">
         <v>0.57284000000000002</v>
       </c>
       <c r="G83" s="6">
@@ -42949,7 +42998,7 @@
       <c r="E84" s="9">
         <v>3.792179</v>
       </c>
-      <c r="F84" s="4">
+      <c r="F84" s="15">
         <v>0.57726</v>
       </c>
       <c r="G84" s="6">
@@ -42972,7 +43021,7 @@
       <c r="E85" s="9">
         <v>3.7276989999999999</v>
       </c>
-      <c r="F85" s="4">
+      <c r="F85" s="15">
         <v>0.58218000000000003</v>
       </c>
       <c r="G85" s="6">
@@ -42995,7 +43044,7 @@
       <c r="E86" s="9">
         <v>3.671081</v>
       </c>
-      <c r="F86" s="4">
+      <c r="F86" s="15">
         <v>0.58750000000000002</v>
       </c>
       <c r="G86" s="6">
@@ -43018,7 +43067,7 @@
       <c r="E87" s="9">
         <v>3.6068370000000001</v>
       </c>
-      <c r="F87" s="4">
+      <c r="F87" s="15">
         <v>0.59165999999999996</v>
       </c>
       <c r="G87" s="6">
@@ -43041,7 +43090,7 @@
       <c r="E88" s="9">
         <v>3.5477240000000001</v>
       </c>
-      <c r="F88" s="4">
+      <c r="F88" s="15">
         <v>0.59465999999999997</v>
       </c>
       <c r="G88" s="6">
@@ -43070,7 +43119,7 @@
       <c r="E89" s="9">
         <v>3.4866760000000001</v>
       </c>
-      <c r="F89" s="4">
+      <c r="F89" s="15">
         <v>0.59836999999999996</v>
       </c>
       <c r="G89" s="6">
@@ -43093,7 +43142,7 @@
       <c r="E90" s="9">
         <v>3.4256600000000001</v>
       </c>
-      <c r="F90" s="4">
+      <c r="F90" s="15">
         <v>0.60368999999999995</v>
       </c>
       <c r="G90" s="6">
@@ -43116,7 +43165,7 @@
       <c r="E91" s="9">
         <v>3.3618209999999999</v>
       </c>
-      <c r="F91" s="4">
+      <c r="F91" s="15">
         <v>0.60775000000000001</v>
       </c>
       <c r="G91" s="6">
@@ -43139,7 +43188,7 @@
       <c r="E92" s="9">
         <v>3.3011889999999999</v>
       </c>
-      <c r="F92" s="4">
+      <c r="F92" s="15">
         <v>0.61436999999999997</v>
       </c>
       <c r="G92" s="6">
@@ -43162,7 +43211,7 @@
       <c r="E93" s="9">
         <v>3.2442709999999999</v>
       </c>
-      <c r="F93" s="4">
+      <c r="F93" s="15">
         <v>0.61573999999999995</v>
       </c>
       <c r="G93" s="6">
@@ -43185,7 +43234,7 @@
       <c r="E94" s="9">
         <v>3.1788430000000001</v>
       </c>
-      <c r="F94" s="4">
+      <c r="F94" s="15">
         <v>0.62033000000000005</v>
       </c>
       <c r="G94" s="6">
@@ -43208,7 +43257,7 @@
       <c r="E95" s="9">
         <v>3.1224219999999998</v>
       </c>
-      <c r="F95" s="4">
+      <c r="F95" s="15">
         <v>0.62273999999999996</v>
       </c>
       <c r="G95" s="6">
@@ -43231,7 +43280,7 @@
       <c r="E96" s="9">
         <v>3.0646</v>
       </c>
-      <c r="F96" s="4">
+      <c r="F96" s="15">
         <v>0.62829999999999997</v>
       </c>
       <c r="G96" s="6">
@@ -43254,7 +43303,7 @@
       <c r="E97" s="9">
         <v>3.0098240000000001</v>
       </c>
-      <c r="F97" s="4">
+      <c r="F97" s="15">
         <v>0.63388999999999995</v>
       </c>
       <c r="G97" s="6">
@@ -43277,7 +43326,7 @@
       <c r="E98" s="9">
         <v>2.9539230000000001</v>
       </c>
-      <c r="F98" s="4">
+      <c r="F98" s="15">
         <v>0.63736999999999999</v>
       </c>
       <c r="G98" s="6">
@@ -43300,7 +43349,7 @@
       <c r="E99" s="9">
         <v>2.9026800000000001</v>
       </c>
-      <c r="F99" s="4">
+      <c r="F99" s="15">
         <v>0.64068999999999998</v>
       </c>
       <c r="G99" s="6">
@@ -43323,7 +43372,7 @@
       <c r="E100" s="9">
         <v>2.8507769999999999</v>
       </c>
-      <c r="F100" s="4">
+      <c r="F100" s="15">
         <v>0.64822000000000002</v>
       </c>
       <c r="G100" s="14">
@@ -43346,7 +43395,7 @@
       <c r="E101" s="9">
         <v>2.8058860000000001</v>
       </c>
-      <c r="F101" s="4">
+      <c r="F101" s="15">
         <v>0.64541000000000004</v>
       </c>
       <c r="G101" s="14">
@@ -43369,7 +43418,7 @@
       <c r="E102" s="9">
         <v>2.7689149999999998</v>
       </c>
-      <c r="F102" s="4">
+      <c r="F102" s="15">
         <v>0.65546000000000004</v>
       </c>
       <c r="G102" s="6">
@@ -43392,7 +43441,7 @@
       <c r="E103" s="9">
         <v>2.7185700000000002</v>
       </c>
-      <c r="F103" s="4">
+      <c r="F103" s="15">
         <v>0.66019000000000005</v>
       </c>
       <c r="G103" s="6">
@@ -43415,7 +43464,7 @@
       <c r="E104" s="9">
         <v>2.6753369999999999</v>
       </c>
-      <c r="F104" s="4">
+      <c r="F104" s="15">
         <v>0.65966000000000002</v>
       </c>
       <c r="G104" s="6">
@@ -43438,7 +43487,7 @@
       <c r="E105" s="9">
         <v>2.6321080000000001</v>
       </c>
-      <c r="F105" s="4">
+      <c r="F105" s="15">
         <v>0.66305000000000003</v>
       </c>
       <c r="G105" s="6">
@@ -43461,7 +43510,7 @@
       <c r="E106" s="9">
         <v>2.5962930000000002</v>
       </c>
-      <c r="F106" s="4">
+      <c r="F106" s="15">
         <v>0.66571999999999998</v>
       </c>
       <c r="G106" s="6">
@@ -43484,7 +43533,7 @@
       <c r="E107" s="9">
         <v>2.5600610000000001</v>
       </c>
-      <c r="F107" s="4">
+      <c r="F107" s="15">
         <v>0.67073000000000005</v>
       </c>
       <c r="G107" s="6">
@@ -43507,7 +43556,7 @@
       <c r="E108" s="9">
         <v>2.5236679999999998</v>
       </c>
-      <c r="F108" s="4">
+      <c r="F108" s="15">
         <v>0.67320000000000002</v>
       </c>
       <c r="G108" s="6">
@@ -43530,7 +43579,7 @@
       <c r="E109" s="9">
         <v>2.485948</v>
       </c>
-      <c r="F109" s="4">
+      <c r="F109" s="15">
         <v>0.67615000000000003</v>
       </c>
       <c r="G109" s="6">
@@ -43553,7 +43602,7 @@
       <c r="E110" s="9">
         <v>2.4536359999999999</v>
       </c>
-      <c r="F110" s="4">
+      <c r="F110" s="15">
         <v>0.68020999999999998</v>
       </c>
       <c r="G110" s="6">
@@ -43576,7 +43625,7 @@
       <c r="E111" s="9">
         <v>2.421732</v>
       </c>
-      <c r="F111" s="6">
+      <c r="F111" s="16">
         <v>0.68376999999999999</v>
       </c>
       <c r="G111" s="6">
@@ -43812,7 +43861,7 @@
       <c r="E121" s="9">
         <v>1.980639</v>
       </c>
-      <c r="F121" s="7">
+      <c r="F121" s="16">
         <v>0.65280000000000005</v>
       </c>
       <c r="G121" s="6">
@@ -43980,7 +44029,7 @@
         <v>0.10231</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -44003,7 +44052,7 @@
         <v>0.10384</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -44026,7 +44075,7 @@
         <v>0.10440000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -44042,799 +44091,1388 @@
       <c r="E131" s="9">
         <v>1.6503410000000001</v>
       </c>
-      <c r="F131" s="7">
+      <c r="F131" s="16">
         <v>0.68942999999999999</v>
       </c>
       <c r="G131" s="6">
         <v>0.1038</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
-      <c r="F132" s="5"/>
-      <c r="G132" s="6"/>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B132" s="9">
+        <v>1.521034</v>
+      </c>
+      <c r="C132" s="9">
+        <v>1.679262</v>
+      </c>
+      <c r="D132" s="9">
+        <v>1.8647670000000001</v>
+      </c>
+      <c r="E132" s="9">
+        <v>1.712413</v>
+      </c>
+      <c r="F132" s="15">
+        <v>0.69579999999999997</v>
+      </c>
+      <c r="G132" s="6">
+        <v>0.10402</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J132" s="1">
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
-      <c r="F133" s="5"/>
-      <c r="G133" s="6"/>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B133" s="9">
+        <v>1.4579949999999999</v>
+      </c>
+      <c r="C133" s="9">
+        <v>1.6021639999999999</v>
+      </c>
+      <c r="D133" s="9">
+        <v>1.763342</v>
+      </c>
+      <c r="E133" s="9">
+        <v>1.6224209999999999</v>
+      </c>
+      <c r="F133" s="15">
+        <v>0.70584999999999998</v>
+      </c>
+      <c r="G133" s="6">
+        <v>0.10562000000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
-      <c r="F134" s="5"/>
-      <c r="G134" s="6"/>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B134" s="17"/>
+      <c r="C134" s="17"/>
+      <c r="D134" s="17"/>
+      <c r="E134" s="17"/>
+      <c r="F134" s="15"/>
+      <c r="G134" s="16"/>
+      <c r="H134" s="17"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>134</v>
       </c>
-      <c r="F135" s="5"/>
-      <c r="G135" s="6"/>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B135" s="17"/>
+      <c r="C135" s="17"/>
+      <c r="D135" s="17"/>
+      <c r="E135" s="17"/>
+      <c r="F135" s="15"/>
+      <c r="G135" s="16"/>
+      <c r="H135" s="17"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
-      <c r="F136" s="5"/>
-      <c r="G136" s="6"/>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B136" s="17"/>
+      <c r="C136" s="17"/>
+      <c r="D136" s="17"/>
+      <c r="E136" s="17"/>
+      <c r="F136" s="15"/>
+      <c r="G136" s="16"/>
+      <c r="H136" s="17"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>136</v>
       </c>
-      <c r="F137" s="5"/>
-      <c r="G137" s="6"/>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B137" s="17"/>
+      <c r="C137" s="17"/>
+      <c r="D137" s="17"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="15"/>
+      <c r="G137" s="16"/>
+      <c r="H137" s="17"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
-      <c r="F138" s="5"/>
-      <c r="G138" s="6"/>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B138" s="17"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="15"/>
+      <c r="G138" s="16"/>
+      <c r="H138" s="17"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
-      <c r="F139" s="6"/>
-      <c r="G139" s="6"/>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B139" s="17"/>
+      <c r="C139" s="17"/>
+      <c r="D139" s="17"/>
+      <c r="E139" s="17"/>
+      <c r="F139" s="16"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="17"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
-      <c r="F140" s="6"/>
-      <c r="G140" s="6"/>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B140" s="17"/>
+      <c r="C140" s="17"/>
+      <c r="D140" s="17"/>
+      <c r="E140" s="17"/>
+      <c r="F140" s="16"/>
+      <c r="G140" s="16"/>
+      <c r="H140" s="17"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
-      <c r="F141" s="7"/>
-      <c r="G141" s="6"/>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B141" s="17"/>
+      <c r="C141" s="17"/>
+      <c r="D141" s="17"/>
+      <c r="E141" s="17"/>
+      <c r="F141" s="16"/>
+      <c r="G141" s="16"/>
+      <c r="H141" s="17"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
-      <c r="F142" s="6"/>
-      <c r="G142" s="6"/>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B142" s="17"/>
+      <c r="C142" s="17"/>
+      <c r="D142" s="17"/>
+      <c r="E142" s="17"/>
+      <c r="F142" s="16"/>
+      <c r="G142" s="16"/>
+      <c r="H142" s="17"/>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
-      <c r="F143" s="6"/>
-      <c r="G143" s="6"/>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B143" s="17"/>
+      <c r="C143" s="17"/>
+      <c r="D143" s="17"/>
+      <c r="E143" s="17"/>
+      <c r="F143" s="16"/>
+      <c r="G143" s="16"/>
+      <c r="H143" s="17"/>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>143</v>
       </c>
-      <c r="F144" s="6"/>
-      <c r="G144" s="6"/>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B144" s="17"/>
+      <c r="C144" s="17"/>
+      <c r="D144" s="17"/>
+      <c r="E144" s="17"/>
+      <c r="F144" s="16"/>
+      <c r="G144" s="16"/>
+      <c r="H144" s="17"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
-      <c r="F145" s="6"/>
-      <c r="G145" s="6"/>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B145" s="17"/>
+      <c r="C145" s="17"/>
+      <c r="D145" s="17"/>
+      <c r="E145" s="17"/>
+      <c r="F145" s="16"/>
+      <c r="G145" s="16"/>
+      <c r="H145" s="17"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
-      <c r="F146" s="6"/>
-      <c r="G146" s="6"/>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B146" s="17"/>
+      <c r="C146" s="17"/>
+      <c r="D146" s="17"/>
+      <c r="E146" s="17"/>
+      <c r="F146" s="16"/>
+      <c r="G146" s="16"/>
+      <c r="H146" s="17"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
-      <c r="F147" s="6"/>
-      <c r="G147" s="6"/>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B147" s="17"/>
+      <c r="C147" s="17"/>
+      <c r="D147" s="17"/>
+      <c r="E147" s="17"/>
+      <c r="F147" s="16"/>
+      <c r="G147" s="16"/>
+      <c r="H147" s="17"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
-      <c r="F148" s="6"/>
-      <c r="G148" s="6"/>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B148" s="17"/>
+      <c r="C148" s="17"/>
+      <c r="D148" s="17"/>
+      <c r="E148" s="17"/>
+      <c r="F148" s="16"/>
+      <c r="G148" s="16"/>
+      <c r="H148" s="17"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
-      <c r="F149" s="6"/>
-      <c r="G149" s="6"/>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B149" s="17"/>
+      <c r="C149" s="17"/>
+      <c r="D149" s="17"/>
+      <c r="E149" s="17"/>
+      <c r="F149" s="16"/>
+      <c r="G149" s="16"/>
+      <c r="H149" s="17"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
-      <c r="F150" s="6"/>
-      <c r="G150" s="6"/>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B150" s="17"/>
+      <c r="C150" s="17"/>
+      <c r="D150" s="17"/>
+      <c r="E150" s="17"/>
+      <c r="F150" s="16"/>
+      <c r="G150" s="16"/>
+      <c r="H150" s="17"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
-      <c r="F151" s="7"/>
-      <c r="G151" s="6"/>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B151" s="17"/>
+      <c r="C151" s="17"/>
+      <c r="D151" s="17"/>
+      <c r="E151" s="17"/>
+      <c r="F151" s="16"/>
+      <c r="G151" s="16"/>
+      <c r="H151" s="17"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
-      <c r="F152" s="6"/>
-      <c r="G152" s="6"/>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B152" s="17"/>
+      <c r="C152" s="17"/>
+      <c r="D152" s="17"/>
+      <c r="E152" s="17"/>
+      <c r="F152" s="16"/>
+      <c r="G152" s="16"/>
+      <c r="H152" s="17"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
-      <c r="F153" s="6"/>
-      <c r="G153" s="6"/>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B153" s="17"/>
+      <c r="C153" s="17"/>
+      <c r="D153" s="17"/>
+      <c r="E153" s="17"/>
+      <c r="F153" s="16"/>
+      <c r="G153" s="16"/>
+      <c r="H153" s="17"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
-      <c r="F154" s="6"/>
-      <c r="G154" s="6"/>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B154" s="17"/>
+      <c r="C154" s="17"/>
+      <c r="D154" s="17"/>
+      <c r="E154" s="17"/>
+      <c r="F154" s="16"/>
+      <c r="G154" s="16"/>
+      <c r="H154" s="17"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
-      <c r="F155" s="6"/>
-      <c r="G155" s="6"/>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B155" s="17"/>
+      <c r="C155" s="17"/>
+      <c r="D155" s="17"/>
+      <c r="E155" s="17"/>
+      <c r="F155" s="16"/>
+      <c r="G155" s="16"/>
+      <c r="H155" s="17"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
-      <c r="F156" s="6"/>
-      <c r="G156" s="6"/>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B156" s="17"/>
+      <c r="C156" s="17"/>
+      <c r="D156" s="17"/>
+      <c r="E156" s="17"/>
+      <c r="F156" s="16"/>
+      <c r="G156" s="16"/>
+      <c r="H156" s="17"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
-      <c r="F157" s="6"/>
-      <c r="G157" s="6"/>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B157" s="17"/>
+      <c r="C157" s="17"/>
+      <c r="D157" s="17"/>
+      <c r="E157" s="17"/>
+      <c r="F157" s="16"/>
+      <c r="G157" s="16"/>
+      <c r="H157" s="17"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
-      <c r="F158" s="6"/>
-      <c r="G158" s="6"/>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B158" s="17"/>
+      <c r="C158" s="17"/>
+      <c r="D158" s="17"/>
+      <c r="E158" s="17"/>
+      <c r="F158" s="16"/>
+      <c r="G158" s="16"/>
+      <c r="H158" s="17"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
-      <c r="F159" s="6"/>
-      <c r="G159" s="6"/>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B159" s="17"/>
+      <c r="C159" s="17"/>
+      <c r="D159" s="17"/>
+      <c r="E159" s="17"/>
+      <c r="F159" s="16"/>
+      <c r="G159" s="16"/>
+      <c r="H159" s="17"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
-      <c r="F160" s="6"/>
-      <c r="G160" s="6"/>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B160" s="17"/>
+      <c r="C160" s="17"/>
+      <c r="D160" s="17"/>
+      <c r="E160" s="17"/>
+      <c r="F160" s="16"/>
+      <c r="G160" s="16"/>
+      <c r="H160" s="17"/>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
-      <c r="F161" s="7"/>
-      <c r="G161" s="6"/>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B161" s="17"/>
+      <c r="C161" s="17"/>
+      <c r="D161" s="17"/>
+      <c r="E161" s="17"/>
+      <c r="F161" s="16"/>
+      <c r="G161" s="16"/>
+      <c r="H161" s="17"/>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
-      <c r="F162" s="6"/>
-      <c r="G162" s="6"/>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B162" s="17"/>
+      <c r="C162" s="17"/>
+      <c r="D162" s="17"/>
+      <c r="E162" s="17"/>
+      <c r="F162" s="16"/>
+      <c r="G162" s="16"/>
+      <c r="H162" s="17"/>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
-      <c r="F163" s="6"/>
-      <c r="G163" s="6"/>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B163" s="17"/>
+      <c r="C163" s="17"/>
+      <c r="D163" s="17"/>
+      <c r="E163" s="17"/>
+      <c r="F163" s="16"/>
+      <c r="G163" s="16"/>
+      <c r="H163" s="17"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
-      <c r="F164" s="6"/>
-      <c r="G164" s="6"/>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B164" s="17"/>
+      <c r="C164" s="17"/>
+      <c r="D164" s="17"/>
+      <c r="E164" s="17"/>
+      <c r="F164" s="16"/>
+      <c r="G164" s="16"/>
+      <c r="H164" s="17"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
-      <c r="F165" s="6"/>
-      <c r="G165" s="6"/>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B165" s="17"/>
+      <c r="C165" s="17"/>
+      <c r="D165" s="17"/>
+      <c r="E165" s="17"/>
+      <c r="F165" s="16"/>
+      <c r="G165" s="16"/>
+      <c r="H165" s="17"/>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
-      <c r="F166" s="6"/>
-      <c r="G166" s="6"/>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B166" s="17"/>
+      <c r="C166" s="17"/>
+      <c r="D166" s="17"/>
+      <c r="E166" s="17"/>
+      <c r="F166" s="16"/>
+      <c r="G166" s="16"/>
+      <c r="H166" s="17"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
-      <c r="F167" s="6"/>
-      <c r="G167" s="6"/>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B167" s="17"/>
+      <c r="C167" s="17"/>
+      <c r="D167" s="17"/>
+      <c r="E167" s="17"/>
+      <c r="F167" s="16"/>
+      <c r="G167" s="16"/>
+      <c r="H167" s="17"/>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
-      <c r="F168" s="6"/>
-      <c r="G168" s="6"/>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B168" s="17"/>
+      <c r="C168" s="17"/>
+      <c r="D168" s="17"/>
+      <c r="E168" s="17"/>
+      <c r="F168" s="16"/>
+      <c r="G168" s="16"/>
+      <c r="H168" s="17"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
-      <c r="F169" s="6"/>
-      <c r="G169" s="6"/>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B169" s="17"/>
+      <c r="C169" s="17"/>
+      <c r="D169" s="17"/>
+      <c r="E169" s="17"/>
+      <c r="F169" s="16"/>
+      <c r="G169" s="16"/>
+      <c r="H169" s="17"/>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
-      <c r="F170" s="6"/>
-      <c r="G170" s="6"/>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B170" s="17"/>
+      <c r="C170" s="17"/>
+      <c r="D170" s="17"/>
+      <c r="E170" s="17"/>
+      <c r="F170" s="16"/>
+      <c r="G170" s="16"/>
+      <c r="H170" s="17"/>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
-      <c r="F171" s="7"/>
-      <c r="G171" s="6"/>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B171" s="17"/>
+      <c r="C171" s="17"/>
+      <c r="D171" s="17"/>
+      <c r="E171" s="17"/>
+      <c r="F171" s="16"/>
+      <c r="G171" s="16"/>
+      <c r="H171" s="17"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
-      <c r="F172" s="6"/>
-      <c r="G172" s="6"/>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B172" s="17"/>
+      <c r="C172" s="17"/>
+      <c r="D172" s="17"/>
+      <c r="E172" s="17"/>
+      <c r="F172" s="16"/>
+      <c r="G172" s="16"/>
+      <c r="H172" s="17"/>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
-      <c r="F173" s="6"/>
-      <c r="G173" s="6"/>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B173" s="17"/>
+      <c r="C173" s="17"/>
+      <c r="D173" s="17"/>
+      <c r="E173" s="17"/>
+      <c r="F173" s="16"/>
+      <c r="G173" s="16"/>
+      <c r="H173" s="17"/>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
-      <c r="F174" s="6"/>
-      <c r="G174" s="6"/>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B174" s="17"/>
+      <c r="C174" s="17"/>
+      <c r="D174" s="17"/>
+      <c r="E174" s="17"/>
+      <c r="F174" s="16"/>
+      <c r="G174" s="16"/>
+      <c r="H174" s="17"/>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
-      <c r="F175" s="6"/>
-      <c r="G175" s="6"/>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B175" s="17"/>
+      <c r="C175" s="17"/>
+      <c r="D175" s="17"/>
+      <c r="E175" s="17"/>
+      <c r="F175" s="16"/>
+      <c r="G175" s="16"/>
+      <c r="H175" s="17"/>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
-      <c r="F176" s="6"/>
-      <c r="G176" s="6"/>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B176" s="17"/>
+      <c r="C176" s="17"/>
+      <c r="D176" s="17"/>
+      <c r="E176" s="17"/>
+      <c r="F176" s="16"/>
+      <c r="G176" s="16"/>
+      <c r="H176" s="17"/>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>176</v>
       </c>
-      <c r="F177" s="6"/>
-      <c r="G177" s="6"/>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B177" s="17"/>
+      <c r="C177" s="17"/>
+      <c r="D177" s="17"/>
+      <c r="E177" s="17"/>
+      <c r="F177" s="16"/>
+      <c r="G177" s="16"/>
+      <c r="H177" s="17"/>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
-      <c r="F178" s="6"/>
-      <c r="G178" s="6"/>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B178" s="17"/>
+      <c r="C178" s="17"/>
+      <c r="D178" s="17"/>
+      <c r="E178" s="17"/>
+      <c r="F178" s="16"/>
+      <c r="G178" s="16"/>
+      <c r="H178" s="17"/>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
-      <c r="F179" s="6"/>
-      <c r="G179" s="6"/>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B179" s="17"/>
+      <c r="C179" s="17"/>
+      <c r="D179" s="17"/>
+      <c r="E179" s="17"/>
+      <c r="F179" s="16"/>
+      <c r="G179" s="16"/>
+      <c r="H179" s="17"/>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
-      <c r="F180" s="6"/>
-      <c r="G180" s="6"/>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B180" s="17"/>
+      <c r="C180" s="17"/>
+      <c r="D180" s="17"/>
+      <c r="E180" s="17"/>
+      <c r="F180" s="16"/>
+      <c r="G180" s="16"/>
+      <c r="H180" s="17"/>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
-      <c r="F181" s="7"/>
-      <c r="G181" s="6"/>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B181" s="17"/>
+      <c r="C181" s="17"/>
+      <c r="D181" s="17"/>
+      <c r="E181" s="17"/>
+      <c r="F181" s="16"/>
+      <c r="G181" s="16"/>
+      <c r="H181" s="17"/>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
-      <c r="F182" s="6"/>
-      <c r="G182" s="6"/>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B182" s="17"/>
+      <c r="C182" s="17"/>
+      <c r="D182" s="17"/>
+      <c r="E182" s="17"/>
+      <c r="F182" s="16"/>
+      <c r="G182" s="16"/>
+      <c r="H182" s="17"/>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>182</v>
       </c>
-      <c r="F183" s="6"/>
-      <c r="G183" s="6"/>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B183" s="17"/>
+      <c r="C183" s="17"/>
+      <c r="D183" s="17"/>
+      <c r="E183" s="17"/>
+      <c r="F183" s="16"/>
+      <c r="G183" s="16"/>
+      <c r="H183" s="17"/>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
-      <c r="F184" s="6"/>
-      <c r="G184" s="6"/>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B184" s="17"/>
+      <c r="C184" s="17"/>
+      <c r="D184" s="17"/>
+      <c r="E184" s="17"/>
+      <c r="F184" s="16"/>
+      <c r="G184" s="16"/>
+      <c r="H184" s="17"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>184</v>
       </c>
-      <c r="F185" s="6"/>
-      <c r="G185" s="6"/>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B185" s="17"/>
+      <c r="C185" s="17"/>
+      <c r="D185" s="17"/>
+      <c r="E185" s="17"/>
+      <c r="F185" s="16"/>
+      <c r="G185" s="16"/>
+      <c r="H185" s="17"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
-      <c r="F186" s="6"/>
-      <c r="G186" s="6"/>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B186" s="17"/>
+      <c r="C186" s="17"/>
+      <c r="D186" s="17"/>
+      <c r="E186" s="17"/>
+      <c r="F186" s="16"/>
+      <c r="G186" s="16"/>
+      <c r="H186" s="17"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>186</v>
       </c>
-      <c r="F187" s="6"/>
-      <c r="G187" s="6"/>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B187" s="17"/>
+      <c r="C187" s="17"/>
+      <c r="D187" s="17"/>
+      <c r="E187" s="17"/>
+      <c r="F187" s="16"/>
+      <c r="G187" s="16"/>
+      <c r="H187" s="17"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
-      <c r="F188" s="6"/>
-      <c r="G188" s="6"/>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B188" s="17"/>
+      <c r="C188" s="17"/>
+      <c r="D188" s="17"/>
+      <c r="E188" s="17"/>
+      <c r="F188" s="16"/>
+      <c r="G188" s="16"/>
+      <c r="H188" s="17"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>188</v>
       </c>
-      <c r="F189" s="6"/>
-      <c r="G189" s="6"/>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B189" s="17"/>
+      <c r="C189" s="17"/>
+      <c r="D189" s="17"/>
+      <c r="E189" s="17"/>
+      <c r="F189" s="16"/>
+      <c r="G189" s="16"/>
+      <c r="H189" s="17"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
-      <c r="F190" s="6"/>
-      <c r="G190" s="6"/>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B190" s="17"/>
+      <c r="C190" s="17"/>
+      <c r="D190" s="17"/>
+      <c r="E190" s="17"/>
+      <c r="F190" s="16"/>
+      <c r="G190" s="16"/>
+      <c r="H190" s="17"/>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>190</v>
       </c>
-      <c r="F191" s="7"/>
-      <c r="G191" s="6"/>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B191" s="17"/>
+      <c r="C191" s="17"/>
+      <c r="D191" s="17"/>
+      <c r="E191" s="17"/>
+      <c r="F191" s="16"/>
+      <c r="G191" s="16"/>
+      <c r="H191" s="17"/>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
-      <c r="F192" s="6"/>
-      <c r="G192" s="6"/>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B192" s="17"/>
+      <c r="C192" s="17"/>
+      <c r="D192" s="17"/>
+      <c r="E192" s="17"/>
+      <c r="F192" s="16"/>
+      <c r="G192" s="16"/>
+      <c r="H192" s="17"/>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
-      <c r="F193" s="6"/>
-      <c r="G193" s="6"/>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B193" s="17"/>
+      <c r="C193" s="17"/>
+      <c r="D193" s="17"/>
+      <c r="E193" s="17"/>
+      <c r="F193" s="16"/>
+      <c r="G193" s="16"/>
+      <c r="H193" s="17"/>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
-      <c r="F194" s="6"/>
-      <c r="G194" s="6"/>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B194" s="17"/>
+      <c r="C194" s="17"/>
+      <c r="D194" s="17"/>
+      <c r="E194" s="17"/>
+      <c r="F194" s="16"/>
+      <c r="G194" s="16"/>
+      <c r="H194" s="17"/>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>194</v>
       </c>
-      <c r="F195" s="6"/>
-      <c r="G195" s="6"/>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B195" s="17"/>
+      <c r="C195" s="17"/>
+      <c r="D195" s="17"/>
+      <c r="E195" s="17"/>
+      <c r="F195" s="16"/>
+      <c r="G195" s="16"/>
+      <c r="H195" s="17"/>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
-      <c r="F196" s="6"/>
-      <c r="G196" s="6"/>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B196" s="17"/>
+      <c r="C196" s="17"/>
+      <c r="D196" s="17"/>
+      <c r="E196" s="17"/>
+      <c r="F196" s="16"/>
+      <c r="G196" s="16"/>
+      <c r="H196" s="17"/>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
-      <c r="F197" s="6"/>
-      <c r="G197" s="6"/>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B197" s="17"/>
+      <c r="C197" s="17"/>
+      <c r="D197" s="17"/>
+      <c r="E197" s="17"/>
+      <c r="F197" s="16"/>
+      <c r="G197" s="16"/>
+      <c r="H197" s="17"/>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
-      <c r="F198" s="6"/>
-      <c r="G198" s="6"/>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B198" s="17"/>
+      <c r="C198" s="17"/>
+      <c r="D198" s="17"/>
+      <c r="E198" s="17"/>
+      <c r="F198" s="16"/>
+      <c r="G198" s="16"/>
+      <c r="H198" s="17"/>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>198</v>
       </c>
-      <c r="F199" s="6"/>
-      <c r="G199" s="6"/>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B199" s="17"/>
+      <c r="C199" s="17"/>
+      <c r="D199" s="17"/>
+      <c r="E199" s="17"/>
+      <c r="F199" s="16"/>
+      <c r="G199" s="16"/>
+      <c r="H199" s="17"/>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
-      <c r="F200" s="6"/>
-      <c r="G200" s="6"/>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B200" s="17"/>
+      <c r="C200" s="17"/>
+      <c r="D200" s="17"/>
+      <c r="E200" s="17"/>
+      <c r="F200" s="16"/>
+      <c r="G200" s="16"/>
+      <c r="H200" s="17"/>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>200</v>
       </c>
-      <c r="F201" s="7"/>
-      <c r="G201" s="6"/>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B201" s="17"/>
+      <c r="C201" s="17"/>
+      <c r="D201" s="17"/>
+      <c r="E201" s="17"/>
+      <c r="F201" s="16"/>
+      <c r="G201" s="16"/>
+      <c r="H201" s="17"/>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
-      <c r="F202" s="6"/>
-      <c r="G202" s="6"/>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B202" s="17"/>
+      <c r="C202" s="17"/>
+      <c r="D202" s="17"/>
+      <c r="E202" s="17"/>
+      <c r="F202" s="16"/>
+      <c r="G202" s="16"/>
+      <c r="H202" s="17"/>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>202</v>
       </c>
-      <c r="F203" s="6"/>
-      <c r="G203" s="6"/>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B203" s="17"/>
+      <c r="C203" s="17"/>
+      <c r="D203" s="17"/>
+      <c r="E203" s="17"/>
+      <c r="F203" s="16"/>
+      <c r="G203" s="16"/>
+      <c r="H203" s="17"/>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
-      <c r="F204" s="6"/>
-      <c r="G204" s="6"/>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B204" s="17"/>
+      <c r="C204" s="17"/>
+      <c r="D204" s="17"/>
+      <c r="E204" s="17"/>
+      <c r="F204" s="16"/>
+      <c r="G204" s="16"/>
+      <c r="H204" s="17"/>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>204</v>
       </c>
-      <c r="F205" s="6"/>
-      <c r="G205" s="6"/>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B205" s="17"/>
+      <c r="C205" s="17"/>
+      <c r="D205" s="17"/>
+      <c r="E205" s="17"/>
+      <c r="F205" s="16"/>
+      <c r="G205" s="16"/>
+      <c r="H205" s="17"/>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>205</v>
       </c>
-      <c r="F206" s="6"/>
-      <c r="G206" s="6"/>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B206" s="17"/>
+      <c r="C206" s="17"/>
+      <c r="D206" s="17"/>
+      <c r="E206" s="17"/>
+      <c r="F206" s="16"/>
+      <c r="G206" s="16"/>
+      <c r="H206" s="17"/>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>206</v>
       </c>
-      <c r="F207" s="6"/>
-      <c r="G207" s="6"/>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B207" s="17"/>
+      <c r="C207" s="17"/>
+      <c r="D207" s="17"/>
+      <c r="E207" s="17"/>
+      <c r="F207" s="16"/>
+      <c r="G207" s="16"/>
+      <c r="H207" s="17"/>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>207</v>
       </c>
-      <c r="F208" s="6"/>
-      <c r="G208" s="6"/>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B208" s="17"/>
+      <c r="C208" s="17"/>
+      <c r="D208" s="17"/>
+      <c r="E208" s="17"/>
+      <c r="F208" s="16"/>
+      <c r="G208" s="16"/>
+      <c r="H208" s="17"/>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>208</v>
       </c>
-      <c r="F209" s="6"/>
-      <c r="G209" s="6"/>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B209" s="17"/>
+      <c r="C209" s="17"/>
+      <c r="D209" s="17"/>
+      <c r="E209" s="17"/>
+      <c r="F209" s="16"/>
+      <c r="G209" s="16"/>
+      <c r="H209" s="17"/>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>209</v>
       </c>
-      <c r="F210" s="7"/>
-      <c r="G210" s="6"/>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B210" s="17"/>
+      <c r="C210" s="17"/>
+      <c r="D210" s="17"/>
+      <c r="E210" s="17"/>
+      <c r="F210" s="16"/>
+      <c r="G210" s="16"/>
+      <c r="H210" s="17"/>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>210</v>
       </c>
-      <c r="F211" s="7"/>
-      <c r="G211" s="6"/>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B211" s="17"/>
+      <c r="C211" s="17"/>
+      <c r="D211" s="17"/>
+      <c r="E211" s="17"/>
+      <c r="F211" s="16"/>
+      <c r="G211" s="16"/>
+      <c r="H211" s="17"/>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>211</v>
       </c>
-      <c r="F212" s="6"/>
-      <c r="G212" s="6"/>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B212" s="17"/>
+      <c r="C212" s="17"/>
+      <c r="D212" s="17"/>
+      <c r="E212" s="17"/>
+      <c r="F212" s="16"/>
+      <c r="G212" s="16"/>
+      <c r="H212" s="17"/>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>212</v>
       </c>
-      <c r="F213" s="6"/>
-      <c r="G213" s="6"/>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B213" s="17"/>
+      <c r="C213" s="17"/>
+      <c r="D213" s="17"/>
+      <c r="E213" s="17"/>
+      <c r="F213" s="16"/>
+      <c r="G213" s="16"/>
+      <c r="H213" s="17"/>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>213</v>
       </c>
-      <c r="F214" s="6"/>
-      <c r="G214" s="6"/>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B214" s="17"/>
+      <c r="C214" s="17"/>
+      <c r="D214" s="17"/>
+      <c r="E214" s="17"/>
+      <c r="F214" s="16"/>
+      <c r="G214" s="16"/>
+      <c r="H214" s="17"/>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>214</v>
       </c>
-      <c r="F215" s="6"/>
-      <c r="G215" s="6"/>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B215" s="17"/>
+      <c r="C215" s="17"/>
+      <c r="D215" s="17"/>
+      <c r="E215" s="17"/>
+      <c r="F215" s="16"/>
+      <c r="G215" s="16"/>
+      <c r="H215" s="17"/>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>215</v>
       </c>
-      <c r="F216" s="6"/>
-      <c r="G216" s="6"/>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B216" s="17"/>
+      <c r="C216" s="17"/>
+      <c r="D216" s="17"/>
+      <c r="E216" s="17"/>
+      <c r="F216" s="16"/>
+      <c r="G216" s="16"/>
+      <c r="H216" s="17"/>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>216</v>
       </c>
-      <c r="F217" s="6"/>
-      <c r="G217" s="6"/>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B217" s="17"/>
+      <c r="C217" s="17"/>
+      <c r="D217" s="17"/>
+      <c r="E217" s="17"/>
+      <c r="F217" s="16"/>
+      <c r="G217" s="16"/>
+      <c r="H217" s="17"/>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>217</v>
       </c>
-      <c r="F218" s="6"/>
-      <c r="G218" s="6"/>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B218" s="17"/>
+      <c r="C218" s="17"/>
+      <c r="D218" s="17"/>
+      <c r="E218" s="17"/>
+      <c r="F218" s="16"/>
+      <c r="G218" s="16"/>
+      <c r="H218" s="17"/>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>218</v>
       </c>
-      <c r="F219" s="6"/>
-      <c r="G219" s="6"/>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B219" s="17"/>
+      <c r="C219" s="17"/>
+      <c r="D219" s="17"/>
+      <c r="E219" s="17"/>
+      <c r="F219" s="16"/>
+      <c r="G219" s="16"/>
+      <c r="H219" s="17"/>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>219</v>
       </c>
-      <c r="F220" s="6"/>
-      <c r="G220" s="6"/>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B220" s="17"/>
+      <c r="C220" s="17"/>
+      <c r="D220" s="17"/>
+      <c r="E220" s="17"/>
+      <c r="F220" s="16"/>
+      <c r="G220" s="16"/>
+      <c r="H220" s="17"/>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>220</v>
       </c>
-      <c r="F221" s="7"/>
-      <c r="G221" s="6"/>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B221" s="17"/>
+      <c r="C221" s="17"/>
+      <c r="D221" s="17"/>
+      <c r="E221" s="17"/>
+      <c r="F221" s="16"/>
+      <c r="G221" s="16"/>
+      <c r="H221" s="17"/>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>221</v>
       </c>
-      <c r="F222" s="6"/>
-      <c r="G222" s="6"/>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B222" s="17"/>
+      <c r="C222" s="17"/>
+      <c r="D222" s="17"/>
+      <c r="E222" s="17"/>
+      <c r="F222" s="16"/>
+      <c r="G222" s="16"/>
+      <c r="H222" s="17"/>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>222</v>
       </c>
-      <c r="F223" s="6"/>
-      <c r="G223" s="6"/>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B223" s="17"/>
+      <c r="C223" s="17"/>
+      <c r="D223" s="17"/>
+      <c r="E223" s="17"/>
+      <c r="F223" s="16"/>
+      <c r="G223" s="16"/>
+      <c r="H223" s="17"/>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>223</v>
       </c>
-      <c r="F224" s="6"/>
-      <c r="G224" s="6"/>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B224" s="17"/>
+      <c r="C224" s="17"/>
+      <c r="D224" s="17"/>
+      <c r="E224" s="17"/>
+      <c r="F224" s="16"/>
+      <c r="G224" s="16"/>
+      <c r="H224" s="17"/>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>224</v>
       </c>
-      <c r="F225" s="6"/>
-      <c r="G225" s="6"/>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B225" s="17"/>
+      <c r="C225" s="17"/>
+      <c r="D225" s="17"/>
+      <c r="E225" s="17"/>
+      <c r="F225" s="16"/>
+      <c r="G225" s="16"/>
+      <c r="H225" s="17"/>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>225</v>
       </c>
-      <c r="F226" s="6"/>
-      <c r="G226" s="6"/>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B226" s="17"/>
+      <c r="C226" s="17"/>
+      <c r="D226" s="17"/>
+      <c r="E226" s="17"/>
+      <c r="F226" s="16"/>
+      <c r="G226" s="16"/>
+      <c r="H226" s="17"/>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>226</v>
       </c>
-      <c r="F227" s="6"/>
-      <c r="G227" s="6"/>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B227" s="17"/>
+      <c r="C227" s="17"/>
+      <c r="D227" s="17"/>
+      <c r="E227" s="17"/>
+      <c r="F227" s="16"/>
+      <c r="G227" s="16"/>
+      <c r="H227" s="17"/>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>227</v>
       </c>
-      <c r="F228" s="6"/>
-      <c r="G228" s="6"/>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B228" s="17"/>
+      <c r="C228" s="17"/>
+      <c r="D228" s="17"/>
+      <c r="E228" s="17"/>
+      <c r="F228" s="16"/>
+      <c r="G228" s="16"/>
+      <c r="H228" s="17"/>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>228</v>
       </c>
-      <c r="F229" s="6"/>
-      <c r="G229" s="6"/>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B229" s="17"/>
+      <c r="C229" s="17"/>
+      <c r="D229" s="17"/>
+      <c r="E229" s="17"/>
+      <c r="F229" s="16"/>
+      <c r="G229" s="16"/>
+      <c r="H229" s="17"/>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>229</v>
       </c>
-      <c r="F230" s="6"/>
-      <c r="G230" s="6"/>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B230" s="17"/>
+      <c r="C230" s="17"/>
+      <c r="D230" s="17"/>
+      <c r="E230" s="17"/>
+      <c r="F230" s="16"/>
+      <c r="G230" s="16"/>
+      <c r="H230" s="17"/>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>230</v>
       </c>
-      <c r="F231" s="7"/>
-      <c r="G231" s="6"/>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B231" s="17"/>
+      <c r="C231" s="17"/>
+      <c r="D231" s="17"/>
+      <c r="E231" s="17"/>
+      <c r="F231" s="16"/>
+      <c r="G231" s="16"/>
+      <c r="H231" s="17"/>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>231</v>
       </c>
-      <c r="F232" s="6"/>
-      <c r="G232" s="6"/>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B232" s="17"/>
+      <c r="C232" s="17"/>
+      <c r="D232" s="17"/>
+      <c r="E232" s="17"/>
+      <c r="F232" s="16"/>
+      <c r="G232" s="16"/>
+      <c r="H232" s="17"/>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>232</v>
       </c>
-      <c r="F233" s="6"/>
-      <c r="G233" s="6"/>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B233" s="17"/>
+      <c r="C233" s="17"/>
+      <c r="D233" s="17"/>
+      <c r="E233" s="17"/>
+      <c r="F233" s="16"/>
+      <c r="G233" s="16"/>
+      <c r="H233" s="17"/>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>233</v>
       </c>
-      <c r="F234" s="6"/>
-      <c r="G234" s="6"/>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B234" s="17"/>
+      <c r="C234" s="17"/>
+      <c r="D234" s="17"/>
+      <c r="E234" s="17"/>
+      <c r="F234" s="16"/>
+      <c r="G234" s="16"/>
+      <c r="H234" s="17"/>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>234</v>
       </c>
-      <c r="F235" s="6"/>
-      <c r="G235" s="6"/>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B235" s="17"/>
+      <c r="C235" s="17"/>
+      <c r="D235" s="17"/>
+      <c r="E235" s="17"/>
+      <c r="F235" s="16"/>
+      <c r="G235" s="16"/>
+      <c r="H235" s="17"/>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>235</v>
       </c>
-      <c r="F236" s="6"/>
-      <c r="G236" s="6"/>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B236" s="17"/>
+      <c r="C236" s="17"/>
+      <c r="D236" s="17"/>
+      <c r="E236" s="17"/>
+      <c r="F236" s="16"/>
+      <c r="G236" s="16"/>
+      <c r="H236" s="17"/>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>236</v>
       </c>
-      <c r="F237" s="6"/>
-      <c r="G237" s="6"/>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B237" s="17"/>
+      <c r="C237" s="17"/>
+      <c r="D237" s="17"/>
+      <c r="E237" s="17"/>
+      <c r="F237" s="16"/>
+      <c r="G237" s="16"/>
+      <c r="H237" s="17"/>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>237</v>
       </c>
-      <c r="F238" s="6"/>
-      <c r="G238" s="6"/>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B238" s="17"/>
+      <c r="C238" s="17"/>
+      <c r="D238" s="17"/>
+      <c r="E238" s="17"/>
+      <c r="F238" s="16"/>
+      <c r="G238" s="16"/>
+      <c r="H238" s="17"/>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>238</v>
       </c>
-      <c r="F239" s="6"/>
-      <c r="G239" s="6"/>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B239" s="17"/>
+      <c r="C239" s="17"/>
+      <c r="D239" s="17"/>
+      <c r="E239" s="17"/>
+      <c r="F239" s="16"/>
+      <c r="G239" s="16"/>
+      <c r="H239" s="17"/>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>239</v>
       </c>
-      <c r="F240" s="6"/>
-      <c r="G240" s="6"/>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B240" s="17"/>
+      <c r="C240" s="17"/>
+      <c r="D240" s="17"/>
+      <c r="E240" s="17"/>
+      <c r="F240" s="16"/>
+      <c r="G240" s="16"/>
+      <c r="H240" s="17"/>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>240</v>
       </c>
-      <c r="F241" s="6"/>
-      <c r="G241" s="6"/>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B241" s="17"/>
+      <c r="C241" s="17"/>
+      <c r="D241" s="17"/>
+      <c r="E241" s="17"/>
+      <c r="F241" s="16"/>
+      <c r="G241" s="16"/>
+      <c r="H241" s="17"/>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>241</v>
       </c>
-      <c r="F242" s="6"/>
-      <c r="G242" s="6"/>
-    </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B242" s="17"/>
+      <c r="C242" s="17"/>
+      <c r="D242" s="17"/>
+      <c r="E242" s="17"/>
+      <c r="F242" s="16"/>
+      <c r="G242" s="16"/>
+      <c r="H242" s="17"/>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>242</v>
       </c>
-      <c r="F243" s="6"/>
-      <c r="G243" s="6"/>
+      <c r="B243" s="17"/>
+      <c r="C243" s="17"/>
+      <c r="D243" s="17"/>
+      <c r="E243" s="17"/>
+      <c r="F243" s="16"/>
+      <c r="G243" s="16"/>
+      <c r="H243" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
~Corrected for bad grammar generation
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\GitHub\auslan-translation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398C1BD5-077C-42A9-89FC-C37765383FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E4BB4C-AD60-48EA-A674-0ABA652D36BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{2BBB440E-AEF7-4CB8-B155-5AEF60BC9E1F}"/>
   </bookViews>
@@ -733,7 +733,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Epoch</t>
   </si>
@@ -844,6 +844,9 @@
   </si>
   <si>
     <t>vocab: 6,808, word-masking: 45,000</t>
+  </si>
+  <si>
+    <t>Regenerated grammar due to error</t>
   </si>
 </sst>
 </file>
@@ -4367,10 +4370,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>noise_grammar_4000!$A$54:$A$156</c:f>
+              <c:f>noise_grammar_4000!$A$54:$A$161</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>53</c:v>
                 </c:pt>
@@ -4679,16 +4682,28 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>noise_grammar_4000!$B$54:$B$156</c:f>
+              <c:f>noise_grammar_4000!$B$54:$B$161</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>5.6611479999999998</c:v>
                 </c:pt>
@@ -4997,6 +5012,18 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>1.214761</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1.8805799999999999</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.4175409999999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.2836689999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.22021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5050,10 +5077,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>noise_grammar_4000!$A$54:$A$156</c:f>
+              <c:f>noise_grammar_4000!$A$54:$A$161</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>53</c:v>
                 </c:pt>
@@ -5362,16 +5389,28 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>noise_grammar_4000!$C$54:$C$156</c:f>
+              <c:f>noise_grammar_4000!$C$54:$C$161</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>5.839899</c:v>
                 </c:pt>
@@ -5680,6 +5719,18 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>1.346204</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.172355</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.5569360000000001</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.4080779999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.3456490000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5719,10 +5770,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>noise_grammar_4000!$A$54:$A$156</c:f>
+              <c:f>noise_grammar_4000!$A$54:$A$161</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>53</c:v>
                 </c:pt>
@@ -6031,16 +6082,28 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>noise_grammar_4000!$D$54:$D$156</c:f>
+              <c:f>noise_grammar_4000!$D$54:$D$161</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>6.294619</c:v>
                 </c:pt>
@@ -6349,6 +6412,18 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>1.4964040000000001</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.6693090000000002</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.7048639999999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.546098</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.486402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6388,10 +6463,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>noise_grammar_4000!$A$54:$A$156</c:f>
+              <c:f>noise_grammar_4000!$A$54:$A$161</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>53</c:v>
                 </c:pt>
@@ -6700,16 +6775,28 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>noise_grammar_4000!$E$54:$E$156</c:f>
+              <c:f>noise_grammar_4000!$E$54:$E$161</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>6.0799709999999996</c:v>
                 </c:pt>
@@ -7018,6 +7105,18 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>1.3693439999999999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.3951090000000002</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.5715779999999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.42961</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.36757</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7087,10 +7186,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>noise_grammar_4000!$A$54:$A$156</c:f>
+              <c:f>noise_grammar_4000!$A$54:$A$161</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>53</c:v>
                 </c:pt>
@@ -7399,16 +7498,28 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>noise_grammar_4000!$F$54:$F$156</c:f>
+              <c:f>noise_grammar_4000!$F$54:$F$161</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>0.48485</c:v>
                 </c:pt>
@@ -7717,6 +7828,18 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>0.74024000000000001</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.65815000000000001</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.71823000000000004</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.73131000000000002</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.75726000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7758,10 +7881,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>noise_grammar_4000!$A$54:$A$156</c:f>
+              <c:f>noise_grammar_4000!$A$54:$A$161</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>53</c:v>
                 </c:pt>
@@ -8070,16 +8193,28 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>noise_grammar_4000!$G$54:$G$156</c:f>
+              <c:f>noise_grammar_4000!$G$54:$G$161</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>0.30924000000000001</c:v>
                 </c:pt>
@@ -8388,6 +8523,18 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>0.11032</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>9.4530000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.10038999999999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.10163999999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.10606</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8619,7 +8766,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
+    <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -41061,10 +41208,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FC3B5E-94BE-4999-BCE6-46D71699FA22}">
-  <dimension ref="A1:AL243"/>
+  <dimension ref="A1:AL244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q54" sqref="Q54"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I159" sqref="I159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44504,7 +44651,7 @@
         <v>0.10829</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -44527,7 +44674,7 @@
         <v>0.10995000000000001</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -44550,7 +44697,7 @@
         <v>0.1085</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -44573,7 +44720,7 @@
         <v>0.10868</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -44596,7 +44743,7 @@
         <v>0.11039</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -44619,7 +44766,7 @@
         <v>0.11111</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -44642,7 +44789,7 @@
         <v>0.1109</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -44665,7 +44812,7 @@
         <v>0.11012</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -44688,7 +44835,7 @@
         <v>0.11018</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -44711,7 +44858,7 @@
         <v>0.10983999999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -44734,7 +44881,7 @@
         <v>0.11002000000000001</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -44757,7 +44904,7 @@
         <v>0.11108999999999999</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -44780,83 +44927,261 @@
         <v>0.11032</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B157" s="9"/>
+      <c r="C157" s="9"/>
+      <c r="D157" s="9"/>
+      <c r="E157" s="9"/>
       <c r="F157" s="6"/>
       <c r="G157" s="6"/>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F158" s="6"/>
-      <c r="G158" s="6"/>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F159" s="6"/>
-      <c r="G159" s="6"/>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F160" s="6"/>
-      <c r="G160" s="6"/>
-    </row>
-    <row r="161" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F161" s="6"/>
-      <c r="G161" s="6"/>
-    </row>
-    <row r="162" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F162" s="6"/>
-      <c r="G162" s="6"/>
-    </row>
-    <row r="163" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F163" s="6"/>
-      <c r="G163" s="6"/>
-    </row>
-    <row r="164" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F164" s="6"/>
-      <c r="G164" s="6"/>
-    </row>
-    <row r="165" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F165" s="6"/>
-      <c r="G165" s="6"/>
-    </row>
-    <row r="166" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F166" s="6"/>
-      <c r="G166" s="6"/>
-    </row>
-    <row r="167" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>146</v>
+      </c>
+      <c r="B158" s="9">
+        <v>1.8805799999999999</v>
+      </c>
+      <c r="C158" s="9">
+        <v>2.172355</v>
+      </c>
+      <c r="D158" s="9">
+        <v>2.6693090000000002</v>
+      </c>
+      <c r="E158" s="9">
+        <v>2.3951090000000002</v>
+      </c>
+      <c r="F158" s="6">
+        <v>0.65815000000000001</v>
+      </c>
+      <c r="G158" s="6">
+        <v>9.4530000000000003E-2</v>
+      </c>
+      <c r="I158" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>147</v>
+      </c>
+      <c r="B159" s="9">
+        <v>1.4175409999999999</v>
+      </c>
+      <c r="C159" s="9">
+        <v>1.5569360000000001</v>
+      </c>
+      <c r="D159" s="9">
+        <v>1.7048639999999999</v>
+      </c>
+      <c r="E159" s="9">
+        <v>1.5715779999999999</v>
+      </c>
+      <c r="F159" s="6">
+        <v>0.71823000000000004</v>
+      </c>
+      <c r="G159" s="6">
+        <v>0.10038999999999999</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>148</v>
+      </c>
+      <c r="B160" s="9">
+        <v>1.2836689999999999</v>
+      </c>
+      <c r="C160" s="9">
+        <v>1.4080779999999999</v>
+      </c>
+      <c r="D160" s="9">
+        <v>1.546098</v>
+      </c>
+      <c r="E160" s="9">
+        <v>1.42961</v>
+      </c>
+      <c r="F160" s="6">
+        <v>0.73131000000000002</v>
+      </c>
+      <c r="G160" s="6">
+        <v>0.10163999999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>149</v>
+      </c>
+      <c r="B161" s="9">
+        <v>1.22021</v>
+      </c>
+      <c r="C161" s="9">
+        <v>1.3456490000000001</v>
+      </c>
+      <c r="D161" s="9">
+        <v>1.486402</v>
+      </c>
+      <c r="E161" s="9">
+        <v>1.36757</v>
+      </c>
+      <c r="F161" s="6">
+        <v>0.75726000000000004</v>
+      </c>
+      <c r="G161" s="6">
+        <v>0.10606</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>150</v>
+      </c>
+      <c r="B162" s="9">
+        <v>1.173243</v>
+      </c>
+      <c r="C162" s="9">
+        <v>1.296289</v>
+      </c>
+      <c r="D162" s="9">
+        <v>1.4334039999999999</v>
+      </c>
+      <c r="E162" s="9">
+        <v>1.3192189999999999</v>
+      </c>
+      <c r="F162" s="6">
+        <v>0.76539000000000001</v>
+      </c>
+      <c r="G162" s="6">
+        <v>0.10685</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>151</v>
+      </c>
+      <c r="B163" s="9">
+        <v>1.140962</v>
+      </c>
+      <c r="C163" s="9">
+        <v>1.263296</v>
+      </c>
+      <c r="D163" s="9">
+        <v>1.400819</v>
+      </c>
+      <c r="E163" s="9">
+        <v>1.2869980000000001</v>
+      </c>
+      <c r="F163" s="6">
+        <v>0.77293999999999996</v>
+      </c>
+      <c r="G163" s="6">
+        <v>0.10835</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>152</v>
+      </c>
+      <c r="B164" s="9">
+        <v>1.108131</v>
+      </c>
+      <c r="C164" s="9">
+        <v>1.2308699999999999</v>
+      </c>
+      <c r="D164" s="9">
+        <v>1.367448</v>
+      </c>
+      <c r="E164" s="9">
+        <v>1.2550319999999999</v>
+      </c>
+      <c r="F164" s="6">
+        <v>0.78191999999999995</v>
+      </c>
+      <c r="G164" s="6">
+        <v>0.10919</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>153</v>
+      </c>
+      <c r="B165" s="9">
+        <v>1.0847869999999999</v>
+      </c>
+      <c r="C165" s="9">
+        <v>1.2056480000000001</v>
+      </c>
+      <c r="D165" s="9">
+        <v>1.3428359999999999</v>
+      </c>
+      <c r="E165" s="9">
+        <v>1.2307319999999999</v>
+      </c>
+      <c r="F165" s="6">
+        <v>0.78693999999999997</v>
+      </c>
+      <c r="G165" s="6">
+        <v>0.11062</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>154</v>
+      </c>
+      <c r="B166" s="9">
+        <v>1.0602819999999999</v>
+      </c>
+      <c r="C166" s="9">
+        <v>1.179209</v>
+      </c>
+      <c r="D166" s="9">
+        <v>1.3163720000000001</v>
+      </c>
+      <c r="E166" s="9">
+        <v>1.2055670000000001</v>
+      </c>
+      <c r="F166" s="6">
+        <v>0.79054000000000002</v>
+      </c>
+      <c r="G166" s="6">
+        <v>0.11123</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F167" s="6"/>
       <c r="G167" s="6"/>
     </row>
-    <row r="168" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F168" s="6"/>
       <c r="G168" s="6"/>
     </row>
-    <row r="169" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F169" s="6"/>
       <c r="G169" s="6"/>
     </row>
-    <row r="170" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F170" s="6"/>
       <c r="G170" s="6"/>
     </row>
-    <row r="171" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F171" s="6"/>
       <c r="G171" s="6"/>
     </row>
-    <row r="172" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F172" s="6"/>
       <c r="G172" s="6"/>
     </row>
-    <row r="173" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F173" s="6"/>
       <c r="G173" s="6"/>
     </row>
-    <row r="174" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F174" s="6"/>
       <c r="G174" s="6"/>
     </row>
-    <row r="175" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F175" s="6"/>
       <c r="G175" s="6"/>
     </row>
-    <row r="176" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F176" s="6"/>
       <c r="G176" s="6"/>
     </row>
@@ -45127,6 +45452,10 @@
     <row r="243" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F243" s="6"/>
       <c r="G243" s="6"/>
+    </row>
+    <row r="244" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F244" s="6"/>
+      <c r="G244" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>